<commit_message>
last edited a month ago
</commit_message>
<xml_diff>
--- a/data/raw_data/Summary_of_primary_data.xlsx
+++ b/data/raw_data/Summary_of_primary_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B882197C-A53A-494F-9790-240E765A6B7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0153B2D4-B9B9-4E05-A8DF-DFDE966FF37B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="10590" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="307">
   <si>
     <t>File_name</t>
   </si>
@@ -519,9 +519,6 @@
     <t>supplementary tables S1-S6</t>
   </si>
   <si>
-    <t>RT-qPCR; proteomics</t>
-  </si>
-  <si>
     <t>Cold stress</t>
   </si>
   <si>
@@ -940,6 +937,12 @@
   </si>
   <si>
     <t>SQD2; DGTT4</t>
+  </si>
+  <si>
+    <t>Only "genes_manipulated that involves over-expression</t>
+  </si>
+  <si>
+    <t>RT_qPCR; proteomics</t>
   </si>
 </sst>
 </file>
@@ -1406,8 +1409,8 @@
   </sheetPr>
   <dimension ref="A1:R56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView tabSelected="1" topLeftCell="L16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1462,22 +1465,22 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O1" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="P1" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
       <c r="R1" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1">
@@ -1627,16 +1630,16 @@
         <v>15</v>
       </c>
       <c r="N4" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>261</v>
+      </c>
+      <c r="P4" t="s">
+        <v>258</v>
+      </c>
+      <c r="Q4" s="21" t="s">
         <v>260</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>262</v>
-      </c>
-      <c r="P4" t="s">
-        <v>259</v>
-      </c>
-      <c r="Q4" s="21" t="s">
-        <v>261</v>
       </c>
       <c r="R4">
         <v>5.5</v>
@@ -2001,10 +2004,10 @@
         <v>15</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>15</v>
@@ -2054,10 +2057,10 @@
         <v>15</v>
       </c>
       <c r="N12" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O12" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P12" s="8" t="s">
         <v>15</v>
@@ -2210,16 +2213,16 @@
         <v>79</v>
       </c>
       <c r="M15" s="21" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="N15" s="21" t="s">
         <v>15</v>
       </c>
       <c r="O15" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P15" s="22" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>15</v>
@@ -2260,7 +2263,7 @@
         <v>15</v>
       </c>
       <c r="L16" s="21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M16" s="8" t="s">
         <v>82</v>
@@ -2372,10 +2375,10 @@
         <v>15</v>
       </c>
       <c r="N18" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="P18" s="8" t="s">
         <v>15</v>
@@ -2431,7 +2434,7 @@
         <v>90</v>
       </c>
       <c r="P19" s="21" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>15</v>
@@ -2478,10 +2481,10 @@
         <v>15</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P20" s="8" t="s">
         <v>15</v>
@@ -2584,10 +2587,10 @@
         <v>15</v>
       </c>
       <c r="N22" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O22" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P22" s="8" t="s">
         <v>15</v>
@@ -2637,10 +2640,10 @@
         <v>15</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="P23" s="8" t="s">
         <v>15</v>
@@ -2690,10 +2693,10 @@
         <v>15</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O24" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P24" s="8" t="s">
         <v>15</v>
@@ -2743,10 +2746,10 @@
         <v>15</v>
       </c>
       <c r="N25" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="O25" s="21" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="P25" s="8" t="s">
         <v>15</v>
@@ -2766,7 +2769,7 @@
         <v>24</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>110</v>
@@ -2902,10 +2905,10 @@
         <v>15</v>
       </c>
       <c r="N28" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O28" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P28" s="8" t="s">
         <v>15</v>
@@ -2952,16 +2955,16 @@
         <v>81</v>
       </c>
       <c r="M29" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="N29" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="O29" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="P29" s="21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="Q29" s="1" t="s">
         <v>126</v>
@@ -3058,19 +3061,19 @@
         <v>81</v>
       </c>
       <c r="M31" t="s">
+        <v>303</v>
+      </c>
+      <c r="N31" s="21" t="s">
         <v>304</v>
       </c>
-      <c r="N31" s="21" t="s">
+      <c r="O31" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="P31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q31" s="1" t="s">
         <v>305</v>
-      </c>
-      <c r="O31" s="21" t="s">
-        <v>295</v>
-      </c>
-      <c r="P31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1">
@@ -3220,10 +3223,10 @@
         <v>15</v>
       </c>
       <c r="N34" s="8" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="P34" s="8" t="s">
         <v>15</v>
@@ -3326,10 +3329,10 @@
         <v>156</v>
       </c>
       <c r="N36" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="P36" s="8" t="s">
         <v>15</v>
@@ -3376,13 +3379,13 @@
         <v>159</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N37" s="8" t="s">
         <v>15</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P37" s="8" t="s">
         <v>15</v>
@@ -3426,27 +3429,27 @@
         <v>15</v>
       </c>
       <c r="L38" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="M38" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="N38" t="s">
+        <v>15</v>
+      </c>
+      <c r="O38" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="P38" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q38" s="1" t="s">
         <v>165</v>
-      </c>
-      <c r="M38" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="N38" t="s">
-        <v>15</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="P38" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="39" spans="1:17" ht="12.75">
       <c r="A39" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>23</v>
@@ -3458,16 +3461,16 @@
         <v>149</v>
       </c>
       <c r="E39" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="F39" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>169</v>
       </c>
       <c r="G39" s="1">
         <v>2015</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I39" s="4">
         <v>43924</v>
@@ -3499,28 +3502,28 @@
     </row>
     <row r="40" spans="1:17" ht="12.75">
       <c r="A40" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D40" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="B40" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" s="1" t="s">
+      <c r="E40" s="3" t="s">
         <v>172</v>
       </c>
-      <c r="E40" s="3" t="s">
+      <c r="F40" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="G40" s="1">
         <v>2013</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="I40" s="4">
         <v>43928</v>
@@ -3547,12 +3550,12 @@
         <v>15</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="41" spans="1:17" ht="12.75">
       <c r="A41" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>23</v>
@@ -3564,7 +3567,7 @@
         <v>161</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="F41" s="1" t="s">
         <v>163</v>
@@ -3573,7 +3576,7 @@
         <v>2014</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="I41" s="4">
         <v>43928</v>
@@ -3600,7 +3603,7 @@
         <v>15</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="42" spans="1:17" ht="12.75">
@@ -3617,7 +3620,7 @@
         <v>49</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>86</v>
@@ -3641,13 +3644,13 @@
         <v>79</v>
       </c>
       <c r="M42" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N42" s="8" t="s">
         <v>15</v>
       </c>
       <c r="O42" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P42" s="8" t="s">
         <v>15</v>
@@ -3658,28 +3661,28 @@
     </row>
     <row r="43" spans="1:17" ht="12.75">
       <c r="A43" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D43" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D43" s="1" t="s">
+      <c r="E43" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="F43" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="G43" s="1">
         <v>2014</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="I43" s="4">
         <v>43934</v>
@@ -3706,33 +3709,33 @@
         <v>15</v>
       </c>
       <c r="Q43" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" spans="1:17" ht="12.75">
       <c r="A44" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B44" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D44" s="1" t="s">
+      <c r="E44" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="F44" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="F44" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="G44" s="1">
         <v>2012</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I44" s="4">
         <v>43934</v>
@@ -3764,7 +3767,7 @@
     </row>
     <row r="45" spans="1:17" ht="12.75">
       <c r="A45" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>23</v>
@@ -3776,10 +3779,10 @@
         <v>87</v>
       </c>
       <c r="E45" s="14" t="s">
+        <v>193</v>
+      </c>
+      <c r="F45" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="G45" s="1">
         <v>2015</v>
@@ -3797,7 +3800,7 @@
         <v>15</v>
       </c>
       <c r="L45" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="M45" s="8" t="s">
         <v>15</v>
@@ -3812,7 +3815,7 @@
         <v>15</v>
       </c>
       <c r="Q45" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="1:17" ht="12.75">
@@ -3826,10 +3829,10 @@
         <v>24</v>
       </c>
       <c r="D46" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>108</v>
@@ -3856,16 +3859,16 @@
         <v>15</v>
       </c>
       <c r="N46" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O46" s="21" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="P46" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q46" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="47" spans="1:17" ht="12.75">
@@ -3882,10 +3885,10 @@
         <v>100</v>
       </c>
       <c r="E47" s="14" t="s">
+        <v>198</v>
+      </c>
+      <c r="F47" s="1" t="s">
         <v>199</v>
-      </c>
-      <c r="F47" s="1" t="s">
-        <v>200</v>
       </c>
       <c r="G47" s="1">
         <v>2016</v>
@@ -3909,10 +3912,10 @@
         <v>15</v>
       </c>
       <c r="N47" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P47" s="8" t="s">
         <v>15</v>
@@ -3923,28 +3926,28 @@
     </row>
     <row r="48" spans="1:17" ht="12.75">
       <c r="A48" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="B48" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="1" t="s">
+      <c r="E48" s="14" t="s">
         <v>202</v>
       </c>
-      <c r="E48" s="14" t="s">
+      <c r="F48" s="1" t="s">
         <v>203</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>204</v>
       </c>
       <c r="G48" s="1">
         <v>2014</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="I48" s="4">
         <v>43935</v>
@@ -3988,10 +3991,10 @@
         <v>87</v>
       </c>
       <c r="E49" s="14" t="s">
+        <v>205</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>206</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>207</v>
       </c>
       <c r="G49" s="1">
         <v>2016</v>
@@ -4012,19 +4015,19 @@
         <v>159</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="N49" s="8" t="s">
         <v>15</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="P49" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q49" s="21" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="R49">
         <v>5.5</v>
@@ -4044,10 +4047,10 @@
         <v>149</v>
       </c>
       <c r="E50" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="F50" s="1" t="s">
         <v>208</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>209</v>
       </c>
       <c r="G50" s="1">
         <v>2017</v>
@@ -4068,19 +4071,19 @@
         <v>159</v>
       </c>
       <c r="M50" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="N50" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O50" s="16" t="s">
+        <v>255</v>
+      </c>
+      <c r="P50" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q50" s="21" t="s">
         <v>256</v>
-      </c>
-      <c r="N50" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O50" s="16" t="s">
-        <v>256</v>
-      </c>
-      <c r="P50" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q50" s="21" t="s">
-        <v>257</v>
       </c>
       <c r="R50">
         <v>5.5</v>
@@ -4088,28 +4091,28 @@
     </row>
     <row r="51" spans="1:18" ht="12.75">
       <c r="A51" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B51" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D51" s="1" t="s">
+      <c r="E51" s="17" t="s">
         <v>211</v>
       </c>
-      <c r="E51" s="17" t="s">
+      <c r="F51" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>213</v>
       </c>
       <c r="G51" s="1">
         <v>2016</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="I51" s="4">
         <v>43935</v>
@@ -4121,16 +4124,16 @@
         <v>15</v>
       </c>
       <c r="L51" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="M51" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N51" s="8" t="s">
         <v>215</v>
       </c>
-      <c r="M51" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N51" s="8" t="s">
-        <v>216</v>
-      </c>
       <c r="O51" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="P51" s="8" t="s">
         <v>15</v>
@@ -4148,13 +4151,13 @@
         <v>24</v>
       </c>
       <c r="D52" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="E52" s="18" t="s">
         <v>217</v>
       </c>
-      <c r="E52" s="18" t="s">
+      <c r="F52" s="1" t="s">
         <v>218</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>219</v>
       </c>
       <c r="G52" s="1">
         <v>2014</v>
@@ -4178,16 +4181,16 @@
         <v>15</v>
       </c>
       <c r="N52" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="O52" s="25" t="s">
+        <v>264</v>
+      </c>
+      <c r="P52" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q52" t="s">
         <v>265</v>
-      </c>
-      <c r="O52" s="25" t="s">
-        <v>265</v>
-      </c>
-      <c r="P52" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>266</v>
       </c>
       <c r="R52">
         <v>5.5</v>
@@ -4204,13 +4207,13 @@
         <v>24</v>
       </c>
       <c r="D53" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E53" s="14" t="s">
         <v>220</v>
       </c>
-      <c r="E53" s="14" t="s">
+      <c r="F53" s="1" t="s">
         <v>221</v>
-      </c>
-      <c r="F53" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="G53" s="1">
         <v>2014</v>
@@ -4231,19 +4234,19 @@
         <v>103</v>
       </c>
       <c r="M53" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="N53" s="16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O53" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="P53" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q53" s="21" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="R53">
         <v>5.5</v>
@@ -4263,10 +4266,10 @@
         <v>56</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="G54" s="1">
         <v>2011</v>
@@ -4287,19 +4290,19 @@
         <v>103</v>
       </c>
       <c r="M54" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="N54" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="O54" s="23" t="s">
+        <v>266</v>
+      </c>
+      <c r="P54" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q54" s="23" t="s">
         <v>267</v>
-      </c>
-      <c r="N54" s="23" t="s">
-        <v>267</v>
-      </c>
-      <c r="O54" s="23" t="s">
-        <v>267</v>
-      </c>
-      <c r="P54" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q54" s="23" t="s">
-        <v>268</v>
       </c>
       <c r="R54">
         <v>5.5</v>
@@ -4316,13 +4319,13 @@
         <v>24</v>
       </c>
       <c r="D55" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="E55" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="F55" s="1" t="s">
         <v>225</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>226</v>
       </c>
       <c r="G55" s="1">
         <v>2014</v>
@@ -4343,17 +4346,17 @@
         <v>79</v>
       </c>
       <c r="M55" s="21" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="N55" s="21" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="O55" s="21" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P55" s="8"/>
       <c r="Q55" s="1" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="R55">
         <v>5.5</v>
@@ -4373,10 +4376,10 @@
         <v>56</v>
       </c>
       <c r="E56" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="F56" s="3" t="s">
         <v>228</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>229</v>
       </c>
       <c r="G56" s="1">
         <v>2016</v>
@@ -4397,13 +4400,13 @@
         <v>65</v>
       </c>
       <c r="M56" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="N56" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O56" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="P56" s="19"/>
     </row>
@@ -4491,27 +4494,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="21" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="21" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="21" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
   </sheetData>
@@ -4537,148 +4540,148 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="27" t="s">
+        <v>277</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>278</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>279</v>
-      </c>
       <c r="C1" s="27" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D1" s="27" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E1" s="27" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="28" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C2" s="27">
         <v>5.5</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="28" t="s">
+        <v>271</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>272</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>273</v>
       </c>
       <c r="C3" s="27">
         <v>5.5</v>
       </c>
       <c r="E3" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="27" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B4" s="28" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C4" s="27">
         <v>5.5</v>
       </c>
       <c r="E4" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="28" t="s">
+        <v>275</v>
+      </c>
+      <c r="B5" s="28" t="s">
         <v>276</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>277</v>
       </c>
       <c r="C5" s="27">
         <v>5.5</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="B6" s="30" t="s">
         <v>280</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>281</v>
       </c>
       <c r="C6" s="27">
         <v>5.5</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="28" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C7" s="27">
         <v>5.5</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>288</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>289</v>
       </c>
       <c r="C8" s="27">
         <v>5.5</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="28" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>290</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>291</v>
       </c>
       <c r="C9" s="27">
         <v>5.5</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="28" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C10" s="27">
         <v>5.5</v>
       </c>
       <c r="D10" s="27" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="11" spans="1:5">

</xml_diff>

<commit_message>
double check genes_manipulated for nonselective_studies; will continue this  tomorrow
</commit_message>
<xml_diff>
--- a/data/raw_data/Summary_of_primary_data.xlsx
+++ b/data/raw_data/Summary_of_primary_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0153B2D4-B9B9-4E05-A8DF-DFDE966FF37B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A813511-E7C9-42C8-B480-ADC95810799F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="10590" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="307">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="304">
   <si>
     <t>File_name</t>
   </si>
@@ -735,21 +735,12 @@
     <t>STA1; STA6</t>
   </si>
   <si>
-    <t>ICL1; MAS1; TAL1; FBP1; PCK1; STA6</t>
-  </si>
-  <si>
     <t>gene_knockout</t>
   </si>
   <si>
     <t>PDAT1</t>
   </si>
   <si>
-    <t xml:space="preserve"> CBF5; FEA1; CTR2; ZRT2</t>
-  </si>
-  <si>
-    <t>DGTT1; DGAT1; PDAT1; NRR1; AMT1D</t>
-  </si>
-  <si>
     <t>DGAT1; DGTT2; DGTT5; ACT1; COX4; COX12</t>
   </si>
   <si>
@@ -915,9 +906,6 @@
     <t xml:space="preserve">Cannot fing GPAT2 in Sato_2014 on Phytozome12, so looked up G3P acyltransferase on Phytozome12 --&gt; used GPA2 gene </t>
   </si>
   <si>
-    <t>DGTT1; DGAT1; PDAT1; NRR1; AMT1D; CBF5; FEA1; CTR2; ZRT2</t>
-  </si>
-  <si>
     <t>Found STA7 on BioCyc; gene synonym = ISA1; look up ISA7 on Phytozome12</t>
   </si>
   <si>
@@ -943,6 +931,9 @@
   </si>
   <si>
     <t>RT_qPCR; proteomics</t>
+  </si>
+  <si>
+    <t>knock_out; transcriptomics</t>
   </si>
 </sst>
 </file>
@@ -952,7 +943,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm\-dd\-yyyy"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1016,12 +1007,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <u/>
@@ -1107,7 +1092,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -1115,27 +1100,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1172,22 +1142,19 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1407,10 +1374,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:R56"/>
+  <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1465,10 +1432,10 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="O1" t="s">
         <v>232</v>
@@ -1480,7 +1447,7 @@
         <v>12</v>
       </c>
       <c r="R1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1">
@@ -1540,22 +1507,22 @@
       <c r="A3" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="8" t="s">
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>25</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="1">
         <v>2013</v>
       </c>
       <c r="H3" s="8" t="s">
@@ -1564,55 +1531,58 @@
       <c r="I3" s="4">
         <v>43914</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="K3" s="1" t="s">
         <v>20</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>21</v>
+        <v>303</v>
       </c>
       <c r="M3" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>15</v>
+        <v>256</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="P3" s="21" t="s">
-        <v>15</v>
+        <v>258</v>
+      </c>
+      <c r="P3" t="s">
+        <v>255</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>15</v>
+        <v>257</v>
+      </c>
+      <c r="R3">
+        <v>5.5</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1">
       <c r="A4" s="21" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="I4" s="4">
         <v>43914</v>
@@ -1623,31 +1593,28 @@
       <c r="K4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="L4" s="21" t="s">
-        <v>65</v>
+      <c r="L4" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="M4" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>259</v>
+        <v>15</v>
       </c>
       <c r="O4" s="21" t="s">
-        <v>261</v>
-      </c>
-      <c r="P4" t="s">
-        <v>258</v>
-      </c>
-      <c r="Q4" s="21" t="s">
-        <v>260</v>
-      </c>
-      <c r="R4">
-        <v>5.5</v>
+        <v>15</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A5" s="21" t="s">
-        <v>29</v>
+      <c r="A5" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>30</v>
@@ -1659,16 +1626,16 @@
         <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G5" s="1">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I5" s="4">
         <v>43914</v>
@@ -1688,43 +1655,43 @@
       <c r="N5" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="O5" s="21" t="s">
+      <c r="O5" s="1" t="s">
         <v>15</v>
       </c>
       <c r="P5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>32</v>
+        <v>42</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="2">
+        <v>779</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="G6" s="1">
-        <v>2017</v>
+        <v>2015</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="I6" s="4">
-        <v>43914</v>
+        <v>43915</v>
       </c>
       <c r="J6" s="1" t="s">
         <v>19</v>
@@ -1748,33 +1715,33 @@
         <v>15</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="2">
-        <v>779</v>
+        <v>48</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="I7" s="4">
         <v>43915</v>
@@ -1806,28 +1773,28 @@
     </row>
     <row r="8" spans="1:18" ht="15.75" customHeight="1">
       <c r="A8" s="1" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>50</v>
+        <v>15</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1">
-        <v>2010</v>
+        <v>2015</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="I8" s="4">
         <v>43915</v>
@@ -1839,7 +1806,7 @@
         <v>20</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="M8" s="21" t="s">
         <v>15</v>
@@ -1854,33 +1821,33 @@
         <v>15</v>
       </c>
       <c r="Q8" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>15</v>
+        <v>56</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G9" s="1">
-        <v>2015</v>
+        <v>2017</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="I9" s="4">
         <v>43915</v>
@@ -1892,7 +1859,7 @@
         <v>20</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="M9" s="21" t="s">
         <v>15</v>
@@ -1907,12 +1874,12 @@
         <v>15</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>23</v>
@@ -1921,46 +1888,46 @@
         <v>24</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="G10" s="1">
-        <v>2017</v>
+        <v>2011</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="I10" s="4">
         <v>43915</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="L10" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="M10" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O10" s="1" t="s">
-        <v>15</v>
+        <v>247</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>247</v>
       </c>
       <c r="P10" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="15.75" customHeight="1">
@@ -1974,16 +1941,16 @@
         <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>62</v>
+        <v>66</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="G11" s="1">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>15</v>
@@ -2004,10 +1971,10 @@
         <v>15</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="O11" s="21" t="s">
-        <v>250</v>
+        <v>233</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>15</v>
@@ -2017,66 +1984,66 @@
       </c>
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>66</v>
+      <c r="A12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G12" s="1">
+        <v>71</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" s="8">
         <v>2009</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="8" t="s">
         <v>15</v>
       </c>
       <c r="I12" s="4">
         <v>43915</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="8" t="s">
         <v>15</v>
       </c>
       <c r="L12" s="5" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="M12" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N12" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="O12" s="21" t="s">
-        <v>233</v>
+      <c r="N12" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>74</v>
       </c>
       <c r="P12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q12" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="8" t="s">
+      <c r="Q12" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" ht="12.75">
+      <c r="A13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D13" s="7" t="s">
@@ -2085,46 +2052,46 @@
       <c r="E13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="8" t="s">
+      <c r="F13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="1">
         <v>2009</v>
       </c>
-      <c r="H13" s="8" t="s">
-        <v>15</v>
+      <c r="H13" s="6" t="s">
+        <v>73</v>
       </c>
       <c r="I13" s="4">
         <v>43915</v>
       </c>
-      <c r="J13" s="8" t="s">
+      <c r="J13" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="K13" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="L13" s="5" t="s">
-        <v>103</v>
+      <c r="K13" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L13" s="21" t="s">
+        <v>112</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N13" s="8" t="s">
-        <v>74</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>74</v>
+        <v>242</v>
+      </c>
+      <c r="N13" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O13" s="21" t="s">
+        <v>15</v>
       </c>
       <c r="P13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q13" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" ht="13.15" thickBot="1">
+      <c r="Q13" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>23</v>
@@ -2132,23 +2099,23 @@
       <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>70</v>
+      <c r="D14" s="21" t="s">
+        <v>80</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="G14" s="1">
-        <v>2009</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>73</v>
+        <v>2012</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="I14" s="4">
-        <v>43915</v>
+        <v>43916</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>64</v>
@@ -2157,27 +2124,27 @@
         <v>15</v>
       </c>
       <c r="L14" s="21" t="s">
-        <v>112</v>
+        <v>237</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N14" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O14" s="21" t="s">
-        <v>15</v>
+      <c r="N14" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="O14" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="P14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" ht="15.75" customHeight="1" thickBot="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>15</v>
+        <v>83</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>23</v>
@@ -2198,7 +2165,7 @@
         <v>2012</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I15" s="4">
         <v>43916</v>
@@ -2212,17 +2179,17 @@
       <c r="L15" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M15" s="21" t="s">
-        <v>297</v>
-      </c>
-      <c r="N15" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O15" s="21" t="s">
-        <v>241</v>
-      </c>
-      <c r="P15" s="22" t="s">
-        <v>240</v>
+      <c r="M15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P15" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="Q15" s="1" t="s">
         <v>15</v>
@@ -2239,22 +2206,22 @@
         <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="G16" s="1">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="4">
-        <v>43916</v>
+        <v>43917</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>64</v>
@@ -2262,17 +2229,17 @@
       <c r="K16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="21" t="s">
-        <v>238</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>82</v>
+      <c r="L16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M16" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N16" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="O16" s="21" t="s">
+        <v>234</v>
       </c>
       <c r="P16" s="8" t="s">
         <v>15</v>
@@ -2283,7 +2250,7 @@
     </row>
     <row r="17" spans="1:17" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>23</v>
@@ -2292,22 +2259,22 @@
         <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>76</v>
+        <v>87</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>77</v>
+        <v>88</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>78</v>
+        <v>89</v>
       </c>
       <c r="G17" s="1">
         <v>2012</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="I17" s="4">
-        <v>43916</v>
+        <v>43917</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>64</v>
@@ -2315,26 +2282,26 @@
       <c r="K17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M17" s="8" t="s">
+      <c r="L17" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M17" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N17" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P17" s="8" t="s">
-        <v>15</v>
+        <v>90</v>
+      </c>
+      <c r="O17" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="P17" s="21" t="s">
+        <v>239</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15.75" customHeight="1">
+    <row r="18" spans="1:17" ht="12.75">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -2345,13 +2312,13 @@
         <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="G18" s="1">
         <v>2010</v>
@@ -2375,10 +2342,10 @@
         <v>15</v>
       </c>
       <c r="N18" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="P18" s="8" t="s">
         <v>15</v>
@@ -2398,13 +2365,13 @@
         <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="G19" s="1">
         <v>2012</v>
@@ -2421,26 +2388,26 @@
       <c r="K19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L19" s="5" t="s">
-        <v>79</v>
+      <c r="L19" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="M19" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="O19" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="P19" s="21" t="s">
-        <v>242</v>
+        <v>96</v>
+      </c>
+      <c r="O19" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="Q19" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="12.75">
+    <row r="20" spans="1:17" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -2451,16 +2418,16 @@
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="G20" s="1">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>15</v>
@@ -2481,10 +2448,10 @@
         <v>15</v>
       </c>
       <c r="N20" s="21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="O20" s="21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="P20" s="8" t="s">
         <v>15</v>
@@ -2504,13 +2471,13 @@
         <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="G21" s="1">
         <v>2012</v>
@@ -2527,17 +2494,17 @@
       <c r="K21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L21" s="1" t="s">
-        <v>65</v>
+      <c r="L21" s="21" t="s">
+        <v>103</v>
       </c>
       <c r="M21" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N21" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="O21" s="8" t="s">
-        <v>96</v>
+      <c r="N21" s="21" t="s">
+        <v>238</v>
+      </c>
+      <c r="O21" s="21" t="s">
+        <v>238</v>
       </c>
       <c r="P21" s="8" t="s">
         <v>15</v>
@@ -2557,16 +2524,16 @@
         <v>24</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>99</v>
+        <v>46</v>
       </c>
       <c r="G22" s="1">
-        <v>2011</v>
+        <v>2012</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>15</v>
@@ -2610,16 +2577,16 @@
         <v>24</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
       <c r="G23" s="1">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>15</v>
@@ -2633,17 +2600,17 @@
       <c r="K23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L23" s="21" t="s">
-        <v>103</v>
+      <c r="L23" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="M23" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N23" s="21" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="O23" s="21" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="P23" s="8" t="s">
         <v>15</v>
@@ -2654,7 +2621,7 @@
     </row>
     <row r="24" spans="1:17" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
@@ -2663,19 +2630,19 @@
         <v>24</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>104</v>
+        <v>230</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>46</v>
+        <v>111</v>
       </c>
       <c r="G24" s="1">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I24" s="4">
         <v>43917</v>
@@ -2687,16 +2654,16 @@
         <v>15</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M24" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="M24" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="O24" s="21" t="s">
-        <v>233</v>
+        <v>286</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="P24" s="8" t="s">
         <v>15</v>
@@ -2707,7 +2674,7 @@
     </row>
     <row r="25" spans="1:17" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>23</v>
@@ -2716,19 +2683,19 @@
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="G25" s="1">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
       <c r="I25" s="4">
         <v>43917</v>
@@ -2740,16 +2707,16 @@
         <v>15</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M25" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N25" s="21" t="s">
-        <v>236</v>
-      </c>
-      <c r="O25" s="21" t="s">
-        <v>236</v>
+        <v>117</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="P25" s="8" t="s">
         <v>15</v>
@@ -2760,7 +2727,7 @@
     </row>
     <row r="26" spans="1:17" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
@@ -2768,20 +2735,20 @@
       <c r="C26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="1" t="s">
-        <v>230</v>
+      <c r="D26" s="21" t="s">
+        <v>119</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="G26" s="1">
-        <v>2011</v>
+        <v>2013</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>40</v>
+        <v>122</v>
       </c>
       <c r="I26" s="4">
         <v>43917</v>
@@ -2792,16 +2759,16 @@
       <c r="K26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L26" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N26" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O26" s="1" t="s">
+      <c r="L26" s="21" t="s">
+        <v>303</v>
+      </c>
+      <c r="M26" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N26" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="O26" s="21" t="s">
         <v>15</v>
       </c>
       <c r="P26" s="8" t="s">
@@ -2813,31 +2780,31 @@
     </row>
     <row r="27" spans="1:17" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C27" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="G27" s="1">
-        <v>2016</v>
+        <v>2012</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>116</v>
+        <v>15</v>
       </c>
       <c r="I27" s="4">
-        <v>43917</v>
+        <v>43922</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>64</v>
@@ -2846,51 +2813,51 @@
         <v>15</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N27" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P27" s="8" t="s">
-        <v>15</v>
+        <v>81</v>
+      </c>
+      <c r="M27" t="s">
+        <v>297</v>
+      </c>
+      <c r="N27" t="s">
+        <v>297</v>
+      </c>
+      <c r="O27" t="s">
+        <v>297</v>
+      </c>
+      <c r="P27" s="21" t="s">
+        <v>240</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>15</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:17" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>118</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>24</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="G28" s="1">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="I28" s="4">
-        <v>43917</v>
+        <v>43922</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>64</v>
@@ -2899,16 +2866,16 @@
         <v>15</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M28" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N28" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="O28" s="21" t="s">
-        <v>237</v>
+        <v>133</v>
+      </c>
+      <c r="M28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N28" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O28" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="P28" s="8" t="s">
         <v>15</v>
@@ -2928,16 +2895,16 @@
         <v>24</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>123</v>
+        <v>134</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>125</v>
+        <v>136</v>
       </c>
       <c r="G29" s="1">
-        <v>2012</v>
+        <v>2014</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>15</v>
@@ -2955,24 +2922,24 @@
         <v>81</v>
       </c>
       <c r="M29" t="s">
+        <v>299</v>
+      </c>
+      <c r="N29" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="O29" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q29" s="1" t="s">
         <v>301</v>
-      </c>
-      <c r="N29" t="s">
-        <v>301</v>
-      </c>
-      <c r="O29" t="s">
-        <v>301</v>
-      </c>
-      <c r="P29" s="21" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>23</v>
@@ -2981,31 +2948,31 @@
         <v>24</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="G30" s="1">
-        <v>2015</v>
-      </c>
-      <c r="H30" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="I30" s="4">
+        <v>2014</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I30" s="9">
         <v>43922</v>
       </c>
-      <c r="J30" s="1" t="s">
+      <c r="J30" s="8" t="s">
         <v>64</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>133</v>
+        <v>21</v>
       </c>
       <c r="M30" s="8" t="s">
         <v>15</v>
@@ -3020,12 +2987,12 @@
         <v>15</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>15</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:17" ht="15.75" customHeight="1">
       <c r="A31" s="1" t="s">
-        <v>15</v>
+        <v>142</v>
       </c>
       <c r="B31" s="8" t="s">
         <v>23</v>
@@ -3034,22 +3001,22 @@
         <v>24</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>134</v>
+        <v>87</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>135</v>
+        <v>143</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="G31" s="1">
-        <v>2014</v>
-      </c>
-      <c r="H31" s="1" t="s">
-        <v>15</v>
+        <v>2012</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="I31" s="4">
-        <v>43922</v>
+        <v>43923</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>64</v>
@@ -3058,27 +3025,27 @@
         <v>15</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M31" t="s">
-        <v>303</v>
-      </c>
-      <c r="N31" s="21" t="s">
-        <v>304</v>
-      </c>
-      <c r="O31" s="21" t="s">
-        <v>294</v>
+        <v>112</v>
+      </c>
+      <c r="M31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O31" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="P31" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>305</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:17" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
-        <v>137</v>
+        <v>15</v>
       </c>
       <c r="B32" s="8" t="s">
         <v>23</v>
@@ -3087,51 +3054,51 @@
         <v>24</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>138</v>
+        <v>49</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="G32" s="1">
-        <v>2014</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I32" s="9">
-        <v>43922</v>
-      </c>
-      <c r="J32" s="8" t="s">
+        <v>2003</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I32" s="4">
+        <v>43923</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>64</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>15</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="M32" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>15</v>
+        <v>242</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>15</v>
+        <v>242</v>
       </c>
       <c r="P32" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:17" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="33" spans="1:18" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>142</v>
+        <v>148</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>23</v>
@@ -3140,19 +3107,19 @@
         <v>24</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>87</v>
+        <v>149</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="G33" s="1">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="I33" s="4">
         <v>43923</v>
@@ -3164,7 +3131,7 @@
         <v>15</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="M33" s="8" t="s">
         <v>15</v>
@@ -3179,10 +3146,10 @@
         <v>15</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="34" spans="1:17" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="25.5">
       <c r="A34" s="1" t="s">
         <v>15</v>
       </c>
@@ -3193,16 +3160,16 @@
         <v>24</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>147</v>
+        <v>153</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>154</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="G34" s="1">
-        <v>2003</v>
+        <v>2013</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>15</v>
@@ -3216,17 +3183,17 @@
       <c r="K34" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L34" s="1" t="s">
-        <v>65</v>
+      <c r="L34" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="M34" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N34" s="8" t="s">
-        <v>245</v>
+        <v>156</v>
+      </c>
+      <c r="N34" s="21" t="s">
+        <v>233</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>245</v>
+        <v>296</v>
       </c>
       <c r="P34" s="8" t="s">
         <v>15</v>
@@ -3235,9 +3202,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:17" ht="15.75" customHeight="1">
+    <row r="35" spans="1:18" ht="12.75">
       <c r="A35" s="1" t="s">
-        <v>148</v>
+        <v>15</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>23</v>
@@ -3246,19 +3213,19 @@
         <v>24</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>158</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>151</v>
+        <v>111</v>
       </c>
       <c r="G35" s="1">
-        <v>2015</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>152</v>
+        <v>2013</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="I35" s="4">
         <v>43923</v>
@@ -3269,17 +3236,17 @@
       <c r="K35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L35" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M35" s="8" t="s">
-        <v>15</v>
+      <c r="L35" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="M35" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="N35" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O35" s="1" t="s">
-        <v>15</v>
+      <c r="O35" s="5" t="s">
+        <v>243</v>
       </c>
       <c r="P35" s="8" t="s">
         <v>15</v>
@@ -3288,9 +3255,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:17" ht="25.5">
+    <row r="36" spans="1:18" ht="12.75">
       <c r="A36" s="1" t="s">
-        <v>15</v>
+        <v>160</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>23</v>
@@ -3299,19 +3266,19 @@
         <v>24</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>154</v>
+        <v>161</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="G36" s="1">
         <v>2013</v>
       </c>
-      <c r="H36" s="1" t="s">
-        <v>15</v>
+      <c r="H36" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="I36" s="4">
         <v>43923</v>
@@ -3322,28 +3289,28 @@
       <c r="K36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L36" s="5" t="s">
-        <v>79</v>
+      <c r="L36" s="1" t="s">
+        <v>302</v>
       </c>
       <c r="M36" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="N36" s="21" t="s">
-        <v>233</v>
+        <v>245</v>
+      </c>
+      <c r="N36" t="s">
+        <v>15</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>300</v>
+        <v>246</v>
       </c>
       <c r="P36" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:17" ht="12.75">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="12.75">
       <c r="A37" s="1" t="s">
-        <v>15</v>
+        <v>166</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>23</v>
@@ -3352,22 +3319,22 @@
         <v>24</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E37" s="11" t="s">
-        <v>158</v>
+        <v>149</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>167</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="G37" s="1">
-        <v>2013</v>
-      </c>
-      <c r="H37" s="1" t="s">
-        <v>15</v>
+        <v>2015</v>
+      </c>
+      <c r="H37" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="I37" s="4">
-        <v>43923</v>
+        <v>43924</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>64</v>
@@ -3375,17 +3342,17 @@
       <c r="K37" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L37" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>246</v>
+      <c r="L37" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M37" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="N37" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O37" s="5" t="s">
-        <v>246</v>
+      <c r="O37" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="P37" s="8" t="s">
         <v>15</v>
@@ -3394,9 +3361,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:17" ht="12.75">
+    <row r="38" spans="1:18" ht="12.75">
       <c r="A38" s="1" t="s">
-        <v>160</v>
+        <v>170</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>23</v>
@@ -3405,22 +3372,22 @@
         <v>24</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>161</v>
+        <v>171</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
       <c r="G38" s="1">
         <v>2013</v>
       </c>
-      <c r="H38" s="6" t="s">
-        <v>164</v>
+      <c r="H38" s="1" t="s">
+        <v>174</v>
       </c>
       <c r="I38" s="4">
-        <v>43923</v>
+        <v>43928</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>64</v>
@@ -3429,27 +3396,27 @@
         <v>15</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>306</v>
+        <v>21</v>
       </c>
       <c r="M38" s="8" t="s">
-        <v>248</v>
-      </c>
-      <c r="N38" t="s">
+        <v>15</v>
+      </c>
+      <c r="N38" s="8" t="s">
         <v>15</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>249</v>
+        <v>15</v>
       </c>
       <c r="P38" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="39" spans="1:17" ht="12.75">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="12.75">
       <c r="A39" s="1" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>23</v>
@@ -3458,22 +3425,22 @@
         <v>24</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G39" s="1">
-        <v>2015</v>
-      </c>
-      <c r="H39" s="12" t="s">
-        <v>169</v>
+        <v>2014</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>178</v>
       </c>
       <c r="I39" s="4">
-        <v>43924</v>
+        <v>43928</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>64</v>
@@ -3482,7 +3449,7 @@
         <v>15</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
       <c r="M39" s="8" t="s">
         <v>15</v>
@@ -3497,12 +3464,12 @@
         <v>15</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:17" ht="12.75">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" ht="12.75">
       <c r="A40" s="1" t="s">
-        <v>170</v>
+        <v>15</v>
       </c>
       <c r="B40" s="8" t="s">
         <v>23</v>
@@ -3511,19 +3478,19 @@
         <v>24</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>171</v>
+        <v>49</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>173</v>
+        <v>86</v>
       </c>
       <c r="G40" s="1">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>174</v>
+        <v>15</v>
       </c>
       <c r="I40" s="4">
         <v>43928</v>
@@ -3534,28 +3501,28 @@
       <c r="K40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L40" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M40" s="8" t="s">
-        <v>15</v>
+      <c r="L40" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M40" s="7" t="s">
+        <v>244</v>
       </c>
       <c r="N40" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O40" s="1" t="s">
-        <v>15</v>
+      <c r="O40" s="7" t="s">
+        <v>244</v>
       </c>
       <c r="P40" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q40" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="41" spans="1:17" ht="12.75">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" ht="12.75">
       <c r="A41" s="1" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>23</v>
@@ -3564,22 +3531,22 @@
         <v>24</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="G41" s="1">
         <v>2014</v>
       </c>
-      <c r="H41" s="1" t="s">
-        <v>178</v>
+      <c r="H41" s="6" t="s">
+        <v>185</v>
       </c>
       <c r="I41" s="4">
-        <v>43928</v>
+        <v>43934</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>64</v>
@@ -3603,12 +3570,12 @@
         <v>15</v>
       </c>
       <c r="Q41" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="42" spans="1:17" ht="12.75">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18" ht="12.75">
       <c r="A42" s="1" t="s">
-        <v>15</v>
+        <v>187</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>23</v>
@@ -3617,22 +3584,22 @@
         <v>24</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>49</v>
+        <v>188</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>86</v>
+        <v>190</v>
       </c>
       <c r="G42" s="1">
         <v>2012</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>15</v>
+        <v>191</v>
       </c>
       <c r="I42" s="4">
-        <v>43928</v>
+        <v>43934</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>64</v>
@@ -3640,17 +3607,17 @@
       <c r="K42" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L42" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="M42" s="7" t="s">
-        <v>247</v>
+      <c r="L42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="M42" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="N42" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O42" s="7" t="s">
-        <v>247</v>
+      <c r="O42" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="P42" s="8" t="s">
         <v>15</v>
@@ -3659,9 +3626,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="43" spans="1:17" ht="12.75">
+    <row r="43" spans="1:18" ht="12.75">
       <c r="A43" s="1" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>23</v>
@@ -3670,19 +3637,19 @@
         <v>24</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>183</v>
+        <v>87</v>
+      </c>
+      <c r="E43" s="14" t="s">
+        <v>193</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>184</v>
+        <v>194</v>
       </c>
       <c r="G43" s="1">
-        <v>2014</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>185</v>
+        <v>2015</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="I43" s="4">
         <v>43934</v>
@@ -3693,8 +3660,8 @@
       <c r="K43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L43" s="1" t="s">
-        <v>112</v>
+      <c r="L43" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="M43" s="8" t="s">
         <v>15</v>
@@ -3712,9 +3679,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="44" spans="1:17" ht="12.75">
+    <row r="44" spans="1:18" ht="12.75">
       <c r="A44" s="1" t="s">
-        <v>187</v>
+        <v>15</v>
       </c>
       <c r="B44" s="8" t="s">
         <v>23</v>
@@ -3723,19 +3690,19 @@
         <v>24</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>190</v>
+        <v>108</v>
       </c>
       <c r="G44" s="1">
-        <v>2012</v>
+        <v>2013</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>191</v>
+        <v>15</v>
       </c>
       <c r="I44" s="4">
         <v>43934</v>
@@ -3747,27 +3714,27 @@
         <v>15</v>
       </c>
       <c r="L44" s="1" t="s">
-        <v>112</v>
+        <v>65</v>
       </c>
       <c r="M44" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N44" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O44" s="8" t="s">
-        <v>15</v>
+      <c r="N44" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="O44" s="21" t="s">
+        <v>233</v>
       </c>
       <c r="P44" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="45" spans="1:17" ht="12.75">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="45" spans="1:18" ht="12.75">
       <c r="A45" s="1" t="s">
-        <v>192</v>
+        <v>15</v>
       </c>
       <c r="B45" s="8" t="s">
         <v>23</v>
@@ -3776,22 +3743,22 @@
         <v>24</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="G45" s="1">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="I45" s="4">
-        <v>43934</v>
+        <v>43935</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>64</v>
@@ -3799,28 +3766,28 @@
       <c r="K45" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L45" s="5" t="s">
-        <v>195</v>
+      <c r="L45" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="M45" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N45" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O45" s="8" t="s">
-        <v>15</v>
+      <c r="N45" t="s">
+        <v>248</v>
+      </c>
+      <c r="O45" s="1" t="s">
+        <v>248</v>
       </c>
       <c r="P45" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q45" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="46" spans="1:17" ht="12.75">
+      <c r="Q45" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18" ht="12.75">
       <c r="A46" s="1" t="s">
-        <v>15</v>
+        <v>200</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>23</v>
@@ -3829,22 +3796,22 @@
         <v>24</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E46" s="3" t="s">
-        <v>197</v>
+        <v>201</v>
+      </c>
+      <c r="E46" s="14" t="s">
+        <v>202</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>108</v>
+        <v>203</v>
       </c>
       <c r="G46" s="1">
-        <v>2013</v>
+        <v>2014</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>15</v>
+        <v>204</v>
       </c>
       <c r="I46" s="4">
-        <v>43934</v>
+        <v>43935</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>64</v>
@@ -3853,25 +3820,25 @@
         <v>15</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>65</v>
+        <v>112</v>
       </c>
       <c r="M46" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N46" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="O46" s="21" t="s">
-        <v>233</v>
+      <c r="N46" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O46" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="P46" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q46" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="47" spans="1:17" ht="12.75">
+      <c r="Q46" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="12.75">
       <c r="A47" s="1" t="s">
         <v>15</v>
       </c>
@@ -3882,13 +3849,13 @@
         <v>24</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="E47" s="14" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="G47" s="1">
         <v>2016</v>
@@ -3905,28 +3872,31 @@
       <c r="K47" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L47" s="1" t="s">
-        <v>65</v>
+      <c r="L47" s="5" t="s">
+        <v>159</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N47" t="s">
-        <v>251</v>
-      </c>
-      <c r="O47" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
+      </c>
+      <c r="N47" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O47" s="2" t="s">
+        <v>250</v>
       </c>
       <c r="P47" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q47" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:17" ht="12.75">
+      <c r="Q47" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="R47">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="12.75">
       <c r="A48" s="1" t="s">
-        <v>200</v>
+        <v>15</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>23</v>
@@ -3935,19 +3905,19 @@
         <v>24</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E48" s="14" t="s">
-        <v>202</v>
+        <v>149</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>207</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="G48" s="1">
-        <v>2014</v>
+        <v>2017</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>204</v>
+        <v>15</v>
       </c>
       <c r="I48" s="4">
         <v>43935</v>
@@ -3958,28 +3928,31 @@
       <c r="K48" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L48" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M48" s="8" t="s">
-        <v>15</v>
+      <c r="L48" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="M48" s="16" t="s">
+        <v>252</v>
       </c>
       <c r="N48" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O48" s="8" t="s">
-        <v>15</v>
+      <c r="O48" s="16" t="s">
+        <v>252</v>
       </c>
       <c r="P48" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q48" s="8" t="s">
-        <v>15</v>
+      <c r="Q48" s="21" t="s">
+        <v>253</v>
+      </c>
+      <c r="R48">
+        <v>5.5</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="12.75">
       <c r="A49" s="1" t="s">
-        <v>15</v>
+        <v>209</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>23</v>
@@ -3988,19 +3961,19 @@
         <v>24</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E49" s="14" t="s">
-        <v>205</v>
+        <v>210</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>211</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="G49" s="1">
         <v>2016</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>15</v>
+        <v>213</v>
       </c>
       <c r="I49" s="4">
         <v>43935</v>
@@ -4011,27 +3984,22 @@
       <c r="K49" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L49" s="5" t="s">
-        <v>159</v>
+      <c r="L49" s="1" t="s">
+        <v>214</v>
       </c>
       <c r="M49" s="8" t="s">
-        <v>253</v>
+        <v>15</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O49" s="2" t="s">
-        <v>253</v>
+        <v>215</v>
+      </c>
+      <c r="O49" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="P49" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q49" s="21" t="s">
-        <v>257</v>
-      </c>
-      <c r="R49">
-        <v>5.5</v>
-      </c>
+      <c r="Q49" s="13"/>
     </row>
     <row r="50" spans="1:18" ht="12.75">
       <c r="A50" s="1" t="s">
@@ -4044,22 +4012,22 @@
         <v>24</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>207</v>
+        <v>216</v>
+      </c>
+      <c r="E50" s="18" t="s">
+        <v>217</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>208</v>
+        <v>218</v>
       </c>
       <c r="G50" s="1">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I50" s="4">
-        <v>43935</v>
+        <v>43937</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>64</v>
@@ -4067,23 +4035,23 @@
       <c r="K50" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L50" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="M50" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="N50" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O50" s="16" t="s">
-        <v>255</v>
+      <c r="L50" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="M50" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N50" s="24" t="s">
+        <v>261</v>
+      </c>
+      <c r="O50" s="24" t="s">
+        <v>261</v>
       </c>
       <c r="P50" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q50" s="21" t="s">
-        <v>256</v>
+      <c r="Q50" t="s">
+        <v>262</v>
       </c>
       <c r="R50">
         <v>5.5</v>
@@ -4091,7 +4059,7 @@
     </row>
     <row r="51" spans="1:18" ht="12.75">
       <c r="A51" s="1" t="s">
-        <v>209</v>
+        <v>15</v>
       </c>
       <c r="B51" s="8" t="s">
         <v>23</v>
@@ -4099,23 +4067,23 @@
       <c r="C51" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D51" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>211</v>
+      <c r="D51" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E51" s="14" t="s">
+        <v>220</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="G51" s="1">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>213</v>
+        <v>15</v>
       </c>
       <c r="I51" s="4">
-        <v>43935</v>
+        <v>43937</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>64</v>
@@ -4124,21 +4092,26 @@
         <v>15</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="M51" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N51" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>215</v>
+        <v>103</v>
+      </c>
+      <c r="M51" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="N51" s="16" t="s">
+        <v>252</v>
+      </c>
+      <c r="O51" s="23" t="s">
+        <v>252</v>
       </c>
       <c r="P51" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q51" s="13"/>
+      <c r="Q51" s="21" t="s">
+        <v>249</v>
+      </c>
+      <c r="R51">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="52" spans="1:18" ht="12.75">
       <c r="A52" s="1" t="s">
@@ -4151,16 +4124,16 @@
         <v>24</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E52" s="18" t="s">
-        <v>217</v>
+        <v>56</v>
+      </c>
+      <c r="E52" s="14" t="s">
+        <v>222</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G52" s="1">
-        <v>2014</v>
+        <v>2011</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>15</v>
@@ -4177,20 +4150,20 @@
       <c r="L52" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="M52" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N52" s="25" t="s">
+      <c r="M52" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="N52" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="O52" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="P52" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q52" s="22" t="s">
         <v>264</v>
-      </c>
-      <c r="O52" s="25" t="s">
-        <v>264</v>
-      </c>
-      <c r="P52" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q52" t="s">
-        <v>265</v>
       </c>
       <c r="R52">
         <v>5.5</v>
@@ -4206,14 +4179,14 @@
       <c r="C53" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="20" t="s">
-        <v>219</v>
+      <c r="D53" s="15" t="s">
+        <v>223</v>
       </c>
       <c r="E53" s="14" t="s">
-        <v>220</v>
+        <v>224</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>221</v>
+        <v>225</v>
       </c>
       <c r="G53" s="1">
         <v>2014</v>
@@ -4230,23 +4203,21 @@
       <c r="K53" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L53" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M53" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="N53" s="16" t="s">
-        <v>255</v>
-      </c>
-      <c r="O53" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="P53" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q53" s="21" t="s">
-        <v>252</v>
+      <c r="L53" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M53" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="N53" s="21" t="s">
+        <v>266</v>
+      </c>
+      <c r="O53" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="P53" s="8"/>
+      <c r="Q53" s="1" t="s">
+        <v>226</v>
       </c>
       <c r="R53">
         <v>5.5</v>
@@ -4266,13 +4237,13 @@
         <v>56</v>
       </c>
       <c r="E54" s="14" t="s">
-        <v>222</v>
-      </c>
-      <c r="F54" s="1" t="s">
-        <v>221</v>
+        <v>227</v>
+      </c>
+      <c r="F54" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="G54" s="1">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="H54" s="1" t="s">
         <v>15</v>
@@ -4287,194 +4258,82 @@
         <v>15</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M54" s="23" t="s">
-        <v>266</v>
-      </c>
-      <c r="N54" s="23" t="s">
-        <v>266</v>
-      </c>
-      <c r="O54" s="23" t="s">
-        <v>266</v>
-      </c>
-      <c r="P54" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q54" s="23" t="s">
-        <v>267</v>
-      </c>
-      <c r="R54">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" ht="12.75">
-      <c r="A55" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B55" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C55" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D55" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="E55" s="14" t="s">
-        <v>224</v>
-      </c>
-      <c r="F55" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="G55" s="1">
-        <v>2014</v>
-      </c>
-      <c r="H55" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I55" s="4">
-        <v>43937</v>
-      </c>
-      <c r="J55" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K55" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L55" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="M55" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="N55" s="21" t="s">
-        <v>269</v>
-      </c>
-      <c r="O55" s="21" t="s">
-        <v>268</v>
-      </c>
-      <c r="P55" s="8"/>
-      <c r="Q55" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="R55">
-        <v>5.5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" ht="12.75">
-      <c r="A56" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C56" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D56" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E56" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="F56" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="G56" s="1">
-        <v>2016</v>
-      </c>
-      <c r="H56" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="I56" s="4">
-        <v>43937</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L56" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M56" s="19" t="s">
+      <c r="M54" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="N56" s="19" t="s">
+      <c r="N54" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="O56" s="19" t="s">
+      <c r="O54" s="19" t="s">
         <v>229</v>
       </c>
-      <c r="P56" s="19"/>
+      <c r="P54" s="19"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E5" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E7" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E8" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E10" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E11" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E12" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E14" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="H14" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E15" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="E16" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E17" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E18" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E19" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E20" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E21" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E22" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E23" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E24" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="E25" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E26" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="E27" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E28" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E29" r:id="rId25" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E30" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E31" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="E32" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="H32" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E33" r:id="rId30" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="H33" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="E34" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="E35" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="H35" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="E36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="E37" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="E38" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="H38" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="E39" r:id="rId39" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="E40" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="E41" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="E42" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="E43" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="H43" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="E44" r:id="rId45" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="E45" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="E46" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="E47" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="E48" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="E49" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="E50" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="E51" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="E52" r:id="rId53" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="E53" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="E54" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="E55" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="E56" r:id="rId57" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="E6" r:id="rId58" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E3" r:id="rId59" xr:uid="{53BA014F-68D7-4B4E-90E5-DE1945E153A0}"/>
-    <hyperlink ref="E13" r:id="rId60" xr:uid="{0896B016-0F4A-4186-939D-3E08BDF72736}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E30" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="H31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="H33" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="E34" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E35" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E36" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="H36" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E37" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E38" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="E39" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="E40" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="E41" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="H41" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="E42" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E43" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="E44" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E45" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="E46" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="E47" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="E48" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="E49" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="E50" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="E51" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="E52" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="E53" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="E54" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="E5" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E12" r:id="rId58" xr:uid="{0896B016-0F4A-4186-939D-3E08BDF72736}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId61"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId59"/>
 </worksheet>
 </file>
 
@@ -4494,27 +4353,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="21" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="21" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="21" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="21" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="21" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
     </row>
   </sheetData>
@@ -4532,160 +4391,160 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.19921875" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="9.19921875" style="27"/>
-    <col min="2" max="2" width="20.3984375" style="27" customWidth="1"/>
-    <col min="3" max="3" width="20.1328125" style="27" customWidth="1"/>
-    <col min="4" max="16384" width="9.19921875" style="27"/>
+    <col min="1" max="1" width="9.19921875" style="26"/>
+    <col min="2" max="2" width="20.3984375" style="26" customWidth="1"/>
+    <col min="3" max="3" width="20.1328125" style="26" customWidth="1"/>
+    <col min="4" max="16384" width="9.19921875" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="26" t="s">
+        <v>274</v>
+      </c>
+      <c r="B1" s="26" t="s">
+        <v>275</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>278</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>258</v>
+      </c>
+      <c r="C2" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="27" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="C3" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="26" t="s">
+        <v>271</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>270</v>
+      </c>
+      <c r="C4" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="E4" s="26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="27" t="s">
+        <v>272</v>
+      </c>
+      <c r="B5" s="27" t="s">
+        <v>273</v>
+      </c>
+      <c r="C5" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="27" t="s">
+        <v>276</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>277</v>
       </c>
-      <c r="B1" s="27" t="s">
-        <v>278</v>
-      </c>
-      <c r="C1" s="27" t="s">
-        <v>254</v>
-      </c>
-      <c r="D1" s="27" t="s">
-        <v>281</v>
-      </c>
-      <c r="E1" s="27" t="s">
+      <c r="C6" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="D6" s="26" t="s">
+        <v>279</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="B7" s="21" t="s">
+        <v>280</v>
+      </c>
+      <c r="C7" s="26">
+        <v>5.5</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="27" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>261</v>
-      </c>
-      <c r="C2" s="27">
+      <c r="B8" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="C8" s="26">
         <v>5.5</v>
       </c>
-      <c r="E2" s="27" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
-      <c r="A3" s="28" t="s">
-        <v>271</v>
-      </c>
-      <c r="B3" s="29" t="s">
-        <v>272</v>
-      </c>
-      <c r="C3" s="27">
+      <c r="E8" s="26" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="27" t="s">
+        <v>286</v>
+      </c>
+      <c r="B9" s="25" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9" s="26">
         <v>5.5</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="27" t="s">
-        <v>274</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>273</v>
-      </c>
-      <c r="C4" s="27">
+      <c r="D9" s="25" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="27" t="s">
+        <v>233</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>290</v>
+      </c>
+      <c r="C10" s="26">
         <v>5.5</v>
       </c>
-      <c r="E4" s="27" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="B5" s="28" t="s">
-        <v>276</v>
-      </c>
-      <c r="C5" s="27">
-        <v>5.5</v>
-      </c>
-      <c r="E5" s="27" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="28" t="s">
-        <v>279</v>
-      </c>
-      <c r="B6" s="30" t="s">
-        <v>280</v>
-      </c>
-      <c r="C6" s="27">
-        <v>5.5</v>
-      </c>
-      <c r="D6" s="27" t="s">
-        <v>282</v>
-      </c>
-      <c r="E6" s="27" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="28" t="s">
-        <v>286</v>
-      </c>
-      <c r="B7" s="21" t="s">
-        <v>283</v>
-      </c>
-      <c r="C7" s="27">
-        <v>5.5</v>
-      </c>
-      <c r="E7" s="27" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="28" t="s">
-        <v>287</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>288</v>
-      </c>
-      <c r="C8" s="27">
-        <v>5.5</v>
-      </c>
-      <c r="E8" s="27" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="28" t="s">
+      <c r="D10" s="26" t="s">
         <v>289</v>
       </c>
-      <c r="B9" s="26" t="s">
-        <v>290</v>
-      </c>
-      <c r="C9" s="27">
-        <v>5.5</v>
-      </c>
-      <c r="D9" s="26" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>293</v>
-      </c>
-      <c r="C10" s="27">
-        <v>5.5</v>
-      </c>
-      <c r="D10" s="27" t="s">
-        <v>292</v>
-      </c>
     </row>
     <row r="11" spans="1:5">
-      <c r="D11" s="31"/>
+      <c r="D11" s="30"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
finish doublechecking Genes_manipulated for nonselective studies
</commit_message>
<xml_diff>
--- a/data/raw_data/Summary_of_primary_data.xlsx
+++ b/data/raw_data/Summary_of_primary_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A813511-E7C9-42C8-B480-ADC95810799F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAF1118-9F87-4625-A6DF-1B6FB6BB00D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="10590" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="303">
   <si>
     <t>File_name</t>
   </si>
@@ -733,9 +733,6 @@
   </si>
   <si>
     <t>STA1; STA6</t>
-  </si>
-  <si>
-    <t>gene_knockout</t>
   </si>
   <si>
     <t>PDAT1</t>
@@ -1376,8 +1373,8 @@
   </sheetPr>
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1432,10 +1429,10 @@
         <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="O1" t="s">
         <v>232</v>
@@ -1447,7 +1444,7 @@
         <v>12</v>
       </c>
       <c r="R1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1">
@@ -1538,22 +1535,22 @@
         <v>20</v>
       </c>
       <c r="L3" s="21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M3" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N3" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="O3" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="P3" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q3" s="21" t="s">
         <v>256</v>
-      </c>
-      <c r="O3" s="21" t="s">
-        <v>258</v>
-      </c>
-      <c r="P3" t="s">
-        <v>255</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>257</v>
       </c>
       <c r="R3">
         <v>5.5</v>
@@ -1918,10 +1915,10 @@
         <v>15</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="O10" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="P10" s="8" t="s">
         <v>15</v>
@@ -2074,7 +2071,7 @@
         <v>112</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="N13" s="21" t="s">
         <v>15</v>
@@ -2123,8 +2120,8 @@
       <c r="K14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="21" t="s">
-        <v>237</v>
+      <c r="L14" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="M14" s="21" t="s">
         <v>15</v>
@@ -2295,7 +2292,7 @@
         <v>90</v>
       </c>
       <c r="P17" s="21" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>15</v>
@@ -2501,10 +2498,10 @@
         <v>15</v>
       </c>
       <c r="N21" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="O21" s="21" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="P21" s="8" t="s">
         <v>15</v>
@@ -2660,7 +2657,7 @@
         <v>15</v>
       </c>
       <c r="N24" s="21" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>15</v>
@@ -2760,7 +2757,7 @@
         <v>15</v>
       </c>
       <c r="L26" s="21" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="M26" s="21" t="s">
         <v>15</v>
@@ -2816,16 +2813,16 @@
         <v>81</v>
       </c>
       <c r="M27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="N27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="O27" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="P27" s="21" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="Q27" s="1" t="s">
         <v>126</v>
@@ -2922,19 +2919,19 @@
         <v>81</v>
       </c>
       <c r="M29" t="s">
+        <v>298</v>
+      </c>
+      <c r="N29" s="21" t="s">
         <v>299</v>
       </c>
-      <c r="N29" s="21" t="s">
+      <c r="O29" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="P29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q29" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="O29" s="21" t="s">
-        <v>291</v>
-      </c>
-      <c r="P29" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="30" spans="1:17" ht="15.75" customHeight="1">
@@ -2978,7 +2975,7 @@
         <v>15</v>
       </c>
       <c r="N30" s="8" t="s">
-        <v>15</v>
+        <v>233</v>
       </c>
       <c r="O30" s="1" t="s">
         <v>15</v>
@@ -3084,10 +3081,10 @@
         <v>15</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="P32" s="8" t="s">
         <v>15</v>
@@ -3193,7 +3190,7 @@
         <v>233</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="P34" s="8" t="s">
         <v>15</v>
@@ -3240,13 +3237,13 @@
         <v>159</v>
       </c>
       <c r="M35" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="N35" s="8" t="s">
         <v>15</v>
       </c>
       <c r="O35" s="5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="P35" s="8" t="s">
         <v>15</v>
@@ -3290,16 +3287,16 @@
         <v>15</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M36" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="N36" t="s">
+        <v>15</v>
+      </c>
+      <c r="O36" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="N36" t="s">
-        <v>15</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>246</v>
       </c>
       <c r="P36" s="8" t="s">
         <v>15</v>
@@ -3505,13 +3502,13 @@
         <v>79</v>
       </c>
       <c r="M40" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="N40" s="8" t="s">
         <v>15</v>
       </c>
       <c r="O40" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="P40" s="8" t="s">
         <v>15</v>
@@ -3773,10 +3770,10 @@
         <v>15</v>
       </c>
       <c r="N45" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P45" s="8" t="s">
         <v>15</v>
@@ -3826,7 +3823,7 @@
         <v>15</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>15</v>
+        <v>233</v>
       </c>
       <c r="O46" s="8" t="s">
         <v>15</v>
@@ -3876,19 +3873,19 @@
         <v>159</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N47" s="8" t="s">
         <v>15</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P47" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q47" s="21" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="R47">
         <v>5.5</v>
@@ -3932,19 +3929,19 @@
         <v>159</v>
       </c>
       <c r="M48" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="N48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O48" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="P48" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q48" s="21" t="s">
         <v>252</v>
-      </c>
-      <c r="N48" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O48" s="16" t="s">
-        <v>252</v>
-      </c>
-      <c r="P48" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q48" s="21" t="s">
-        <v>253</v>
       </c>
       <c r="R48">
         <v>5.5</v>
@@ -4042,16 +4039,16 @@
         <v>15</v>
       </c>
       <c r="N50" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="O50" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="P50" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q50" t="s">
         <v>261</v>
-      </c>
-      <c r="O50" s="24" t="s">
-        <v>261</v>
-      </c>
-      <c r="P50" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q50" t="s">
-        <v>262</v>
       </c>
       <c r="R50">
         <v>5.5</v>
@@ -4095,19 +4092,19 @@
         <v>103</v>
       </c>
       <c r="M51" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="N51" s="16" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="O51" s="23" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="P51" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q51" s="21" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="R51">
         <v>5.5</v>
@@ -4151,19 +4148,19 @@
         <v>103</v>
       </c>
       <c r="M52" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="N52" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="O52" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="P52" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q52" s="22" t="s">
         <v>263</v>
-      </c>
-      <c r="N52" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="O52" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="P52" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q52" s="22" t="s">
-        <v>264</v>
       </c>
       <c r="R52">
         <v>5.5</v>
@@ -4207,13 +4204,13 @@
         <v>79</v>
       </c>
       <c r="M53" s="21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="N53" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="P53" s="8"/>
       <c r="Q53" s="1" t="s">
@@ -4353,27 +4350,27 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="21" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:1">
       <c r="A3" s="21" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="21" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="5" spans="1:1">
       <c r="A5" s="21" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
   </sheetData>
@@ -4399,134 +4396,134 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="26" t="s">
+        <v>273</v>
+      </c>
+      <c r="B1" s="26" t="s">
         <v>274</v>
       </c>
-      <c r="B1" s="26" t="s">
-        <v>275</v>
-      </c>
       <c r="C1" s="26" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C2" s="26">
         <v>5.5</v>
       </c>
       <c r="E2" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="B3" s="28" t="s">
         <v>268</v>
-      </c>
-      <c r="B3" s="28" t="s">
-        <v>269</v>
       </c>
       <c r="C3" s="26">
         <v>5.5</v>
       </c>
       <c r="E3" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="26" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="C4" s="26">
         <v>5.5</v>
       </c>
       <c r="E4" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="27" t="s">
+        <v>271</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>272</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>273</v>
       </c>
       <c r="C5" s="26">
         <v>5.5</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="27" t="s">
+        <v>275</v>
+      </c>
+      <c r="B6" s="29" t="s">
         <v>276</v>
-      </c>
-      <c r="B6" s="29" t="s">
-        <v>277</v>
       </c>
       <c r="C6" s="26">
         <v>5.5</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C7" s="26">
         <v>5.5</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="27" t="s">
+        <v>283</v>
+      </c>
+      <c r="B8" s="21" t="s">
         <v>284</v>
-      </c>
-      <c r="B8" s="21" t="s">
-        <v>285</v>
       </c>
       <c r="C8" s="26">
         <v>5.5</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="B9" s="25" t="s">
         <v>286</v>
-      </c>
-      <c r="B9" s="25" t="s">
-        <v>287</v>
       </c>
       <c r="C9" s="26">
         <v>5.5</v>
       </c>
       <c r="D9" s="25" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -4534,13 +4531,13 @@
         <v>233</v>
       </c>
       <c r="B10" s="25" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C10" s="26">
         <v>5.5</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="11" spans="1:5">

</xml_diff>

<commit_message>
sorted by author and year; added letter after year to distinguish between rows that have the same author and year
</commit_message>
<xml_diff>
--- a/data/raw_data/Summary_of_primary_data.xlsx
+++ b/data/raw_data/Summary_of_primary_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alice\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DAF1118-9F87-4625-A6DF-1B6FB6BB00D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A4CEDF-1687-4012-A9F4-7840E51B70E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="10590" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="846" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="307">
   <si>
     <t>File_name</t>
   </si>
@@ -931,6 +931,18 @@
   </si>
   <si>
     <t>knock_out; transcriptomics</t>
+  </si>
+  <si>
+    <t>2012a</t>
+  </si>
+  <si>
+    <t>2012b</t>
+  </si>
+  <si>
+    <t>2009a</t>
+  </si>
+  <si>
+    <t>2009b</t>
   </si>
 </sst>
 </file>
@@ -1373,8 +1385,8 @@
   </sheetPr>
   <dimension ref="A1:R54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.46484375" defaultRowHeight="15.75" customHeight="1"/>
@@ -1449,60 +1461,58 @@
     </row>
     <row r="2" spans="1:18" ht="15.75" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>209</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>14</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>16</v>
+        <v>210</v>
+      </c>
+      <c r="E2" s="17" t="s">
+        <v>211</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>212</v>
       </c>
       <c r="G2" s="1">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>18</v>
+        <v>213</v>
       </c>
       <c r="I2" s="4">
-        <v>43914</v>
+        <v>43935</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>21</v>
+        <v>214</v>
       </c>
       <c r="M2" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N2" s="8" t="s">
-        <v>15</v>
+        <v>215</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>15</v>
+        <v>215</v>
       </c>
       <c r="P2" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="Q2" s="13"/>
     </row>
     <row r="3" spans="1:18" ht="15.75" customHeight="1">
       <c r="A3" s="8" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>23</v>
@@ -1510,29 +1520,29 @@
       <c r="C3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>25</v>
+      <c r="D3" s="21" t="s">
+        <v>119</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>26</v>
+        <v>120</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>27</v>
+        <v>121</v>
       </c>
       <c r="G3" s="1">
         <v>2013</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>28</v>
+        <v>122</v>
       </c>
       <c r="I3" s="4">
-        <v>43914</v>
+        <v>43917</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L3" s="21" t="s">
         <v>302</v>
@@ -1541,116 +1551,113 @@
         <v>15</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>255</v>
+        <v>233</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>257</v>
-      </c>
-      <c r="P3" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q3" s="21" t="s">
-        <v>256</v>
-      </c>
-      <c r="R3">
-        <v>5.5</v>
+        <v>15</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="15.75" customHeight="1">
-      <c r="A4" s="21" t="s">
-        <v>29</v>
+      <c r="A4" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>32</v>
+        <v>23</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>80</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2015</v>
+        <v>78</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="I4" s="4">
-        <v>43914</v>
+        <v>43916</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>21</v>
+        <v>15</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>65</v>
       </c>
       <c r="M4" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N4" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="21" t="s">
-        <v>15</v>
+      <c r="N4" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="P4" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>36</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:18" ht="15.75" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>83</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>31</v>
+        <v>23</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>24</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>38</v>
+        <v>77</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="1">
-        <v>2017</v>
+        <v>78</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>304</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I5" s="4">
-        <v>43914</v>
+        <v>43916</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M5" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N5" s="21" t="s">
-        <v>15</v>
+        <v>15</v>
+      </c>
+      <c r="L5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="O5" s="1" t="s">
         <v>15</v>
@@ -1659,54 +1666,54 @@
         <v>15</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>41</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:18" ht="15.75" customHeight="1">
       <c r="A6" s="1" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="2">
-        <v>779</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>45</v>
+        <v>24</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>198</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>46</v>
+        <v>199</v>
       </c>
       <c r="G6" s="1">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="I6" s="4">
-        <v>43915</v>
+        <v>43935</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M6" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N6" s="21" t="s">
-        <v>15</v>
+        <v>65</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N6" t="s">
+        <v>247</v>
       </c>
       <c r="O6" s="1" t="s">
-        <v>15</v>
+        <v>247</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>15</v>
@@ -1717,7 +1724,7 @@
     </row>
     <row r="7" spans="1:18" ht="15.75" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>48</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>23</v>
@@ -1726,46 +1733,49 @@
         <v>24</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>50</v>
+        <v>56</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>222</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>51</v>
+        <v>221</v>
       </c>
       <c r="G7" s="1">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="I7" s="4">
-        <v>43915</v>
+        <v>43937</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N7" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O7" s="1" t="s">
-        <v>15</v>
+        <v>103</v>
+      </c>
+      <c r="M7" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="N7" s="22" t="s">
+        <v>262</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>262</v>
       </c>
       <c r="P7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q7" s="1" t="s">
-        <v>15</v>
+      <c r="Q7" s="22" t="s">
+        <v>263</v>
+      </c>
+      <c r="R7">
+        <v>5.5</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="15.75" customHeight="1">
@@ -1773,57 +1783,60 @@
         <v>15</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="20" t="s">
+        <v>219</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>220</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>53</v>
+        <v>221</v>
       </c>
       <c r="G8" s="1">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="4">
-        <v>43915</v>
+        <v>43937</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="M8" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N8" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O8" s="1" t="s">
-        <v>15</v>
+        <v>103</v>
+      </c>
+      <c r="M8" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="N8" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="O8" s="23" t="s">
+        <v>251</v>
       </c>
       <c r="P8" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q8" s="1" t="s">
-        <v>54</v>
+      <c r="Q8" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="R8">
+        <v>5.5</v>
       </c>
     </row>
     <row r="9" spans="1:18" ht="15.75" customHeight="1">
       <c r="A9" s="1" t="s">
-        <v>55</v>
+        <v>15</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>23</v>
@@ -1832,93 +1845,93 @@
         <v>24</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>57</v>
+        <v>105</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="G9" s="1">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="I9" s="4">
-        <v>43915</v>
+        <v>43917</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>19</v>
+        <v>64</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>21</v>
+        <v>65</v>
       </c>
       <c r="M9" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="O9" s="1" t="s">
-        <v>15</v>
+        <v>233</v>
+      </c>
+      <c r="O9" s="21" t="s">
+        <v>233</v>
       </c>
       <c r="P9" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q9" s="1" t="s">
-        <v>60</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="15.75" customHeight="1">
       <c r="A10" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="6" t="s">
-        <v>62</v>
+        <v>44</v>
+      </c>
+      <c r="D10" s="1">
+        <v>779</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="G10" s="1">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>15</v>
+        <v>47</v>
       </c>
       <c r="I10" s="4">
         <v>43915</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>65</v>
+        <v>20</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="M10" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="O10" s="21" t="s">
-        <v>246</v>
+        <v>15</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="P10" s="8" t="s">
         <v>15</v>
@@ -1929,7 +1942,7 @@
     </row>
     <row r="11" spans="1:18" ht="15.75" customHeight="1">
       <c r="A11" s="1" t="s">
-        <v>15</v>
+        <v>166</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>23</v>
@@ -1938,22 +1951,22 @@
         <v>24</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>66</v>
+        <v>149</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>67</v>
+        <v>167</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>68</v>
+        <v>168</v>
       </c>
       <c r="G11" s="1">
-        <v>2009</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>15</v>
+        <v>2015</v>
+      </c>
+      <c r="H11" s="12" t="s">
+        <v>169</v>
       </c>
       <c r="I11" s="4">
-        <v>43915</v>
+        <v>43924</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>64</v>
@@ -1961,17 +1974,17 @@
       <c r="K11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="M11" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N11" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="O11" s="21" t="s">
-        <v>233</v>
+      <c r="L11" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N11" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O11" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="P11" s="8" t="s">
         <v>15</v>
@@ -1982,7 +1995,7 @@
     </row>
     <row r="12" spans="1:18" ht="15.75" customHeight="1">
       <c r="A12" s="8" t="s">
-        <v>15</v>
+        <v>137</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>23</v>
@@ -1990,23 +2003,23 @@
       <c r="C12" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D12" s="7" t="s">
-        <v>70</v>
+      <c r="D12" s="8" t="s">
+        <v>138</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>71</v>
+        <v>139</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>72</v>
+        <v>140</v>
       </c>
       <c r="G12" s="8">
-        <v>2009</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="I12" s="4">
-        <v>43915</v>
+        <v>2014</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I12" s="9">
+        <v>43922</v>
       </c>
       <c r="J12" s="8" t="s">
         <v>64</v>
@@ -2014,28 +2027,28 @@
       <c r="K12" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="M12" s="21" t="s">
+      <c r="L12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>74</v>
+        <v>233</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>74</v>
+        <v>15</v>
       </c>
       <c r="P12" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>15</v>
+        <v>141</v>
       </c>
     </row>
     <row r="13" spans="1:18" ht="12.75">
       <c r="A13" s="1" t="s">
-        <v>69</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>23</v>
@@ -2043,23 +2056,23 @@
       <c r="C13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="7" t="s">
-        <v>70</v>
+      <c r="D13" s="8" t="s">
+        <v>97</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>71</v>
+        <v>98</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>72</v>
+        <v>99</v>
       </c>
       <c r="G13" s="1">
-        <v>2009</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>73</v>
+        <v>2011</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="I13" s="4">
-        <v>43915</v>
+        <v>43917</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>64</v>
@@ -2067,28 +2080,28 @@
       <c r="K13" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L13" s="21" t="s">
-        <v>112</v>
+      <c r="L13" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="M13" s="21" t="s">
-        <v>241</v>
+        <v>15</v>
       </c>
       <c r="N13" s="21" t="s">
-        <v>15</v>
+        <v>233</v>
       </c>
       <c r="O13" s="21" t="s">
-        <v>15</v>
+        <v>233</v>
       </c>
       <c r="P13" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>75</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="15.75" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>181</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>23</v>
@@ -2096,23 +2109,23 @@
       <c r="C14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D14" s="21" t="s">
-        <v>80</v>
+      <c r="D14" s="8" t="s">
+        <v>182</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>77</v>
+        <v>183</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>78</v>
+        <v>184</v>
       </c>
       <c r="G14" s="1">
-        <v>2012</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>15</v>
+        <v>2014</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>185</v>
       </c>
       <c r="I14" s="4">
-        <v>43916</v>
+        <v>43934</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>64</v>
@@ -2120,67 +2133,67 @@
       <c r="K14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L14" s="5" t="s">
-        <v>65</v>
-      </c>
-      <c r="M14" s="21" t="s">
+      <c r="L14" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N14" s="8" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>82</v>
+        <v>15</v>
       </c>
       <c r="P14" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>15</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="15.75" customHeight="1">
       <c r="A15" s="1" t="s">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>77</v>
+        <v>15</v>
+      </c>
+      <c r="E15" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="G15" s="1">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="I15" s="4">
-        <v>43916</v>
+        <v>43915</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L15" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>82</v>
+        <v>20</v>
+      </c>
+      <c r="L15" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="M15" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N15" s="21" t="s">
+        <v>15</v>
       </c>
       <c r="O15" s="1" t="s">
         <v>15</v>
@@ -2189,7 +2202,7 @@
         <v>15</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>15</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" spans="1:18" ht="15.75" customHeight="1">
@@ -2203,22 +2216,22 @@
         <v>24</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>84</v>
+        <v>134</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>85</v>
+        <v>135</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>86</v>
+        <v>136</v>
       </c>
       <c r="G16" s="1">
-        <v>2010</v>
+        <v>2014</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="4">
-        <v>43917</v>
+        <v>43922</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>64</v>
@@ -2227,25 +2240,25 @@
         <v>15</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M16" s="21" t="s">
-        <v>15</v>
+        <v>81</v>
+      </c>
+      <c r="M16" t="s">
+        <v>298</v>
       </c>
       <c r="N16" s="21" t="s">
-        <v>234</v>
+        <v>299</v>
       </c>
       <c r="O16" s="21" t="s">
-        <v>234</v>
+        <v>290</v>
       </c>
       <c r="P16" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" ht="15.75" customHeight="1">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" ht="15.75" customHeight="1">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2256,16 +2269,16 @@
         <v>24</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="G17" s="1">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>15</v>
@@ -2279,26 +2292,26 @@
       <c r="K17" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L17" s="5" t="s">
-        <v>79</v>
+      <c r="L17" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="M17" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N17" s="8" t="s">
-        <v>90</v>
+      <c r="N17" s="21" t="s">
+        <v>236</v>
       </c>
       <c r="O17" s="21" t="s">
-        <v>90</v>
-      </c>
-      <c r="P17" s="21" t="s">
-        <v>238</v>
+        <v>236</v>
+      </c>
+      <c r="P17" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="Q17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="12.75">
+    <row r="18" spans="1:18" ht="12.75">
       <c r="A18" s="1" t="s">
         <v>15</v>
       </c>
@@ -2309,22 +2322,22 @@
         <v>24</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>91</v>
+        <v>196</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>92</v>
+        <v>197</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="G18" s="1">
-        <v>2010</v>
+        <v>2013</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I18" s="4">
-        <v>43917</v>
+        <v>43934</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>64</v>
@@ -2335,25 +2348,25 @@
       <c r="L18" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="M18" s="21" t="s">
+      <c r="M18" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N18" s="21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="O18" s="21" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="P18" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" ht="15.75" customHeight="1">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="15.75" customHeight="1">
       <c r="A19" s="1" t="s">
-        <v>15</v>
+        <v>148</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>23</v>
@@ -2362,22 +2375,22 @@
         <v>24</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>94</v>
+        <v>149</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>95</v>
+        <v>150</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>86</v>
+        <v>151</v>
       </c>
       <c r="G19" s="1">
-        <v>2012</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>15</v>
+        <v>2015</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>152</v>
       </c>
       <c r="I19" s="4">
-        <v>43917</v>
+        <v>43923</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>64</v>
@@ -2386,16 +2399,16 @@
         <v>15</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M19" s="21" t="s">
+        <v>133</v>
+      </c>
+      <c r="M19" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N19" s="8" t="s">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="O19" s="8" t="s">
-        <v>96</v>
+        <v>15</v>
       </c>
       <c r="P19" s="8" t="s">
         <v>15</v>
@@ -2404,7 +2417,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15.75" customHeight="1">
+    <row r="20" spans="1:18" ht="15.75" customHeight="1">
       <c r="A20" s="1" t="s">
         <v>15</v>
       </c>
@@ -2415,22 +2428,22 @@
         <v>24</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>98</v>
+        <v>207</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>99</v>
+        <v>208</v>
       </c>
       <c r="G20" s="1">
-        <v>2011</v>
+        <v>2017</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I20" s="4">
-        <v>43917</v>
+        <v>43935</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>64</v>
@@ -2438,28 +2451,31 @@
       <c r="K20" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M20" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N20" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="O20" s="21" t="s">
-        <v>233</v>
+      <c r="L20" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="M20" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="N20" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O20" s="16" t="s">
+        <v>251</v>
       </c>
       <c r="P20" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q20" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" ht="15.75" customHeight="1">
+      <c r="Q20" s="21" t="s">
+        <v>252</v>
+      </c>
+      <c r="R20">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15.75" customHeight="1">
       <c r="A21" s="1" t="s">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>23</v>
@@ -2468,49 +2484,49 @@
         <v>24</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>101</v>
+        <v>57</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>102</v>
+        <v>58</v>
       </c>
       <c r="G21" s="1">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>15</v>
+        <v>59</v>
       </c>
       <c r="I21" s="4">
-        <v>43917</v>
+        <v>43915</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L21" s="21" t="s">
-        <v>103</v>
+        <v>20</v>
+      </c>
+      <c r="L21" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="M21" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N21" s="21" t="s">
-        <v>237</v>
-      </c>
-      <c r="O21" s="21" t="s">
-        <v>237</v>
+        <v>15</v>
+      </c>
+      <c r="O21" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="P21" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" ht="15.75" customHeight="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
         <v>15</v>
       </c>
@@ -2521,13 +2537,13 @@
         <v>24</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>46</v>
+        <v>125</v>
       </c>
       <c r="G22" s="1">
         <v>2012</v>
@@ -2536,7 +2552,7 @@
         <v>15</v>
       </c>
       <c r="I22" s="4">
-        <v>43917</v>
+        <v>43922</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>64</v>
@@ -2545,27 +2561,27 @@
         <v>15</v>
       </c>
       <c r="L22" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M22" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N22" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="O22" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="P22" s="8" t="s">
-        <v>15</v>
+        <v>81</v>
+      </c>
+      <c r="M22" t="s">
+        <v>296</v>
+      </c>
+      <c r="N22" t="s">
+        <v>296</v>
+      </c>
+      <c r="O22" t="s">
+        <v>296</v>
+      </c>
+      <c r="P22" s="21" t="s">
+        <v>239</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" customHeight="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" ht="15.75" customHeight="1">
       <c r="A23" s="1" t="s">
-        <v>15</v>
+        <v>142</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>23</v>
@@ -2574,22 +2590,22 @@
         <v>24</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>106</v>
+        <v>87</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>107</v>
+        <v>143</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="G23" s="1">
-        <v>2011</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>15</v>
+        <v>2012</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>145</v>
       </c>
       <c r="I23" s="4">
-        <v>43917</v>
+        <v>43923</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>64</v>
@@ -2598,27 +2614,27 @@
         <v>15</v>
       </c>
       <c r="L23" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M23" s="21" t="s">
-        <v>15</v>
-      </c>
-      <c r="N23" s="21" t="s">
-        <v>236</v>
-      </c>
-      <c r="O23" s="21" t="s">
-        <v>236</v>
+        <v>112</v>
+      </c>
+      <c r="M23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O23" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="P23" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" ht="15.75" customHeight="1">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="15.75" customHeight="1">
       <c r="A24" s="1" t="s">
-        <v>109</v>
+        <v>192</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>23</v>
@@ -2627,22 +2643,22 @@
         <v>24</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>110</v>
+        <v>87</v>
+      </c>
+      <c r="E24" s="14" t="s">
+        <v>193</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>111</v>
+        <v>194</v>
       </c>
       <c r="G24" s="1">
-        <v>2011</v>
+        <v>2015</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>40</v>
       </c>
       <c r="I24" s="4">
-        <v>43917</v>
+        <v>43934</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>64</v>
@@ -2650,14 +2666,14 @@
       <c r="K24" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L24" s="1" t="s">
-        <v>112</v>
+      <c r="L24" s="5" t="s">
+        <v>195</v>
       </c>
       <c r="M24" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N24" s="21" t="s">
-        <v>285</v>
+      <c r="N24" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="O24" s="1" t="s">
         <v>15</v>
@@ -2666,12 +2682,12 @@
         <v>15</v>
       </c>
       <c r="Q24" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" customHeight="1">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" ht="15.75" customHeight="1">
       <c r="A25" s="1" t="s">
-        <v>113</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>23</v>
@@ -2680,19 +2696,19 @@
         <v>24</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>114</v>
+        <v>84</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>115</v>
+        <v>85</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>86</v>
       </c>
       <c r="G25" s="1">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>116</v>
+        <v>15</v>
       </c>
       <c r="I25" s="4">
         <v>43917</v>
@@ -2704,16 +2720,16 @@
         <v>15</v>
       </c>
       <c r="L25" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N25" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>15</v>
+        <v>65</v>
+      </c>
+      <c r="M25" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N25" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="O25" s="21" t="s">
+        <v>234</v>
       </c>
       <c r="P25" s="8" t="s">
         <v>15</v>
@@ -2722,9 +2738,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15.75" customHeight="1">
+    <row r="26" spans="1:18" ht="15.75" customHeight="1">
       <c r="A26" s="1" t="s">
-        <v>118</v>
+        <v>15</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
@@ -2732,20 +2748,20 @@
       <c r="C26" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D26" s="21" t="s">
-        <v>119</v>
+      <c r="D26" s="8" t="s">
+        <v>94</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>120</v>
+        <v>95</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G26" s="1">
-        <v>2013</v>
+        <v>86</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>303</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>122</v>
+        <v>15</v>
       </c>
       <c r="I26" s="4">
         <v>43917</v>
@@ -2756,17 +2772,17 @@
       <c r="K26" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L26" s="21" t="s">
-        <v>302</v>
+      <c r="L26" s="8" t="s">
+        <v>65</v>
       </c>
       <c r="M26" s="21" t="s">
         <v>15</v>
       </c>
-      <c r="N26" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="O26" s="21" t="s">
-        <v>15</v>
+      <c r="N26" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="O26" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="P26" s="8" t="s">
         <v>15</v>
@@ -2775,7 +2791,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15.75" customHeight="1">
+    <row r="27" spans="1:18" ht="15.75" customHeight="1">
       <c r="A27" s="1" t="s">
         <v>15</v>
       </c>
@@ -2786,22 +2802,22 @@
         <v>24</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>123</v>
+        <v>49</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>124</v>
+        <v>180</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="1">
-        <v>2012</v>
+        <v>86</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>304</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I27" s="4">
-        <v>43922</v>
+        <v>43928</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>64</v>
@@ -2809,28 +2825,28 @@
       <c r="K27" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L27" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M27" t="s">
-        <v>296</v>
-      </c>
-      <c r="N27" t="s">
-        <v>296</v>
-      </c>
-      <c r="O27" t="s">
-        <v>296</v>
-      </c>
-      <c r="P27" s="21" t="s">
-        <v>239</v>
+      <c r="L27" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="N27" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="P27" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="Q27" s="1" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" ht="15.75" customHeight="1">
       <c r="A28" s="1" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="B28" s="8" t="s">
         <v>23</v>
@@ -2839,22 +2855,22 @@
         <v>24</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>130</v>
+        <v>115</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>131</v>
+        <v>86</v>
       </c>
       <c r="G28" s="1">
-        <v>2015</v>
+        <v>2016</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="I28" s="4">
-        <v>43922</v>
+        <v>43917</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>64</v>
@@ -2863,7 +2879,7 @@
         <v>15</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="M28" s="8" t="s">
         <v>15</v>
@@ -2881,9 +2897,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15.75" customHeight="1">
+    <row r="29" spans="1:18" ht="15.75" customHeight="1">
       <c r="A29" s="1" t="s">
-        <v>15</v>
+        <v>187</v>
       </c>
       <c r="B29" s="8" t="s">
         <v>23</v>
@@ -2892,22 +2908,22 @@
         <v>24</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>134</v>
+        <v>188</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>135</v>
+        <v>189</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>136</v>
+        <v>190</v>
       </c>
       <c r="G29" s="1">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>15</v>
+        <v>191</v>
       </c>
       <c r="I29" s="4">
-        <v>43922</v>
+        <v>43934</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>64</v>
@@ -2916,27 +2932,27 @@
         <v>15</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M29" t="s">
-        <v>298</v>
-      </c>
-      <c r="N29" s="21" t="s">
-        <v>299</v>
-      </c>
-      <c r="O29" s="21" t="s">
-        <v>290</v>
+        <v>112</v>
+      </c>
+      <c r="M29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O29" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="P29" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q29" s="1" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" ht="15.75" customHeight="1">
       <c r="A30" s="1" t="s">
-        <v>137</v>
+        <v>22</v>
       </c>
       <c r="B30" s="8" t="s">
         <v>23</v>
@@ -2945,89 +2961,92 @@
         <v>24</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>138</v>
+        <v>25</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>139</v>
+        <v>26</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>140</v>
+        <v>27</v>
       </c>
       <c r="G30" s="1">
-        <v>2014</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I30" s="9">
-        <v>43922</v>
+        <v>2013</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I30" s="4">
+        <v>43914</v>
       </c>
       <c r="J30" s="8" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L30" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L30" s="21" t="s">
+        <v>302</v>
+      </c>
+      <c r="M30" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N30" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="O30" s="21" t="s">
+        <v>257</v>
+      </c>
+      <c r="P30" t="s">
+        <v>254</v>
+      </c>
+      <c r="Q30" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="R30">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="15.75" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="1">
+        <v>2010</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" s="4">
+        <v>43915</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L31" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="M30" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N30" s="8" t="s">
-        <v>233</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="P30" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" customHeight="1">
-      <c r="A31" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B31" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C31" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="F31" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="G31" s="1">
-        <v>2012</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="I31" s="4">
-        <v>43923</v>
-      </c>
-      <c r="J31" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L31" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M31" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N31" s="8" t="s">
+      <c r="M31" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N31" s="21" t="s">
         <v>15</v>
       </c>
       <c r="O31" s="1" t="s">
@@ -3037,10 +3056,10 @@
         <v>15</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" customHeight="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="15.75" customHeight="1">
       <c r="A32" s="1" t="s">
         <v>15</v>
       </c>
@@ -3050,23 +3069,23 @@
       <c r="C32" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D32" s="1" t="s">
-        <v>49</v>
+      <c r="D32" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>147</v>
+        <v>71</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="G32" s="1">
-        <v>2003</v>
+        <v>72</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>305</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I32" s="4">
-        <v>43923</v>
+        <v>43915</v>
       </c>
       <c r="J32" s="1" t="s">
         <v>64</v>
@@ -3074,17 +3093,17 @@
       <c r="K32" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L32" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M32" s="8" t="s">
+      <c r="L32" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="M32" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N32" s="8" t="s">
-        <v>241</v>
+        <v>74</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>241</v>
+        <v>74</v>
       </c>
       <c r="P32" s="8" t="s">
         <v>15</v>
@@ -3095,7 +3114,7 @@
     </row>
     <row r="33" spans="1:18" ht="15.75" customHeight="1">
       <c r="A33" s="1" t="s">
-        <v>148</v>
+        <v>69</v>
       </c>
       <c r="B33" s="8" t="s">
         <v>23</v>
@@ -3103,23 +3122,23 @@
       <c r="C33" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D33" s="1" t="s">
-        <v>149</v>
+      <c r="D33" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>150</v>
+        <v>71</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="G33" s="1">
-        <v>2015</v>
+        <v>72</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>306</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>152</v>
+        <v>73</v>
       </c>
       <c r="I33" s="4">
-        <v>43923</v>
+        <v>43915</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>64</v>
@@ -3127,26 +3146,26 @@
       <c r="K33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L33" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M33" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N33" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O33" s="1" t="s">
+      <c r="L33" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="M33" s="21" t="s">
+        <v>241</v>
+      </c>
+      <c r="N33" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O33" s="21" t="s">
         <v>15</v>
       </c>
       <c r="P33" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" ht="25.5">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="12.75">
       <c r="A34" s="1" t="s">
         <v>15</v>
       </c>
@@ -3157,22 +3176,22 @@
         <v>24</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>154</v>
+        <v>87</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>88</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
       <c r="G34" s="1">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I34" s="4">
-        <v>43923</v>
+        <v>43917</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>64</v>
@@ -3183,17 +3202,17 @@
       <c r="L34" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="M34" s="8" t="s">
-        <v>156</v>
-      </c>
-      <c r="N34" s="21" t="s">
-        <v>233</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>295</v>
-      </c>
-      <c r="P34" s="8" t="s">
-        <v>15</v>
+      <c r="M34" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N34" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="O34" s="21" t="s">
+        <v>90</v>
+      </c>
+      <c r="P34" s="21" t="s">
+        <v>238</v>
       </c>
       <c r="Q34" s="1" t="s">
         <v>15</v>
@@ -3201,7 +3220,7 @@
     </row>
     <row r="35" spans="1:18" ht="12.75">
       <c r="A35" s="1" t="s">
-        <v>15</v>
+        <v>109</v>
       </c>
       <c r="B35" s="8" t="s">
         <v>23</v>
@@ -3210,22 +3229,22 @@
         <v>24</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="E35" s="11" t="s">
-        <v>158</v>
+        <v>230</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>110</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>111</v>
       </c>
       <c r="G35" s="1">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>15</v>
+        <v>40</v>
       </c>
       <c r="I35" s="4">
-        <v>43923</v>
+        <v>43917</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>64</v>
@@ -3233,17 +3252,17 @@
       <c r="K35" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L35" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="N35" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O35" s="5" t="s">
-        <v>242</v>
+      <c r="L35" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M35" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N35" s="21" t="s">
+        <v>285</v>
+      </c>
+      <c r="O35" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="P35" s="8" t="s">
         <v>15</v>
@@ -3254,7 +3273,7 @@
     </row>
     <row r="36" spans="1:18" ht="12.75">
       <c r="A36" s="1" t="s">
-        <v>160</v>
+        <v>15</v>
       </c>
       <c r="B36" s="8" t="s">
         <v>23</v>
@@ -3263,19 +3282,19 @@
         <v>24</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>162</v>
+        <v>157</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>158</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>163</v>
+        <v>111</v>
       </c>
       <c r="G36" s="1">
         <v>2013</v>
       </c>
-      <c r="H36" s="6" t="s">
-        <v>164</v>
+      <c r="H36" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="I36" s="4">
         <v>43923</v>
@@ -3286,66 +3305,66 @@
       <c r="K36" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L36" s="1" t="s">
-        <v>301</v>
-      </c>
-      <c r="M36" s="8" t="s">
-        <v>244</v>
-      </c>
-      <c r="N36" t="s">
-        <v>15</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>245</v>
+      <c r="L36" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="M36" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="N36" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O36" s="5" t="s">
+        <v>242</v>
       </c>
       <c r="P36" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>165</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:18" ht="12.75">
       <c r="A37" s="1" t="s">
-        <v>166</v>
+        <v>37</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>149</v>
+        <v>32</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>167</v>
+        <v>38</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>168</v>
+        <v>39</v>
       </c>
       <c r="G37" s="1">
-        <v>2015</v>
-      </c>
-      <c r="H37" s="12" t="s">
-        <v>169</v>
+        <v>2017</v>
+      </c>
+      <c r="H37" s="8" t="s">
+        <v>40</v>
       </c>
       <c r="I37" s="4">
-        <v>43924</v>
+        <v>43914</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L37" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="M37" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N37" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="M37" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N37" s="21" t="s">
         <v>15</v>
       </c>
       <c r="O37" s="8" t="s">
@@ -3355,12 +3374,12 @@
         <v>15</v>
       </c>
       <c r="Q37" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:18" ht="12.75">
       <c r="A38" s="1" t="s">
-        <v>170</v>
+        <v>128</v>
       </c>
       <c r="B38" s="8" t="s">
         <v>23</v>
@@ -3369,22 +3388,22 @@
         <v>24</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>171</v>
+        <v>129</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>172</v>
+        <v>130</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>173</v>
+        <v>131</v>
       </c>
       <c r="G38" s="1">
-        <v>2013</v>
+        <v>2015</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>174</v>
+        <v>132</v>
       </c>
       <c r="I38" s="4">
-        <v>43928</v>
+        <v>43922</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>64</v>
@@ -3393,7 +3412,7 @@
         <v>15</v>
       </c>
       <c r="L38" s="1" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="M38" s="8" t="s">
         <v>15</v>
@@ -3408,12 +3427,12 @@
         <v>15</v>
       </c>
       <c r="Q38" s="1" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" ht="12.75">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" ht="25.5">
       <c r="A39" s="1" t="s">
-        <v>176</v>
+        <v>15</v>
       </c>
       <c r="B39" s="8" t="s">
         <v>23</v>
@@ -3422,22 +3441,22 @@
         <v>24</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>177</v>
+        <v>153</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>154</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="G39" s="1">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>178</v>
+        <v>15</v>
       </c>
       <c r="I39" s="4">
-        <v>43928</v>
+        <v>43923</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>64</v>
@@ -3445,23 +3464,23 @@
       <c r="K39" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L39" s="1" t="s">
-        <v>112</v>
+      <c r="L39" s="5" t="s">
+        <v>79</v>
       </c>
       <c r="M39" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N39" s="8" t="s">
-        <v>15</v>
+        <v>156</v>
+      </c>
+      <c r="N39" s="21" t="s">
+        <v>233</v>
       </c>
       <c r="O39" s="8" t="s">
-        <v>15</v>
+        <v>295</v>
       </c>
       <c r="P39" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q39" s="1" t="s">
-        <v>179</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:18" ht="12.75">
@@ -3478,19 +3497,19 @@
         <v>49</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>180</v>
+        <v>147</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="G40" s="1">
-        <v>2012</v>
+        <v>2003</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I40" s="4">
-        <v>43928</v>
+        <v>43923</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>64</v>
@@ -3498,17 +3517,17 @@
       <c r="K40" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L40" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="M40" s="7" t="s">
-        <v>243</v>
+      <c r="L40" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="M40" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="N40" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O40" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
+      </c>
+      <c r="O40" s="8" t="s">
+        <v>241</v>
       </c>
       <c r="P40" s="8" t="s">
         <v>15</v>
@@ -3519,7 +3538,7 @@
     </row>
     <row r="41" spans="1:18" ht="12.75">
       <c r="A41" s="1" t="s">
-        <v>181</v>
+        <v>15</v>
       </c>
       <c r="B41" s="8" t="s">
         <v>23</v>
@@ -3527,23 +3546,23 @@
       <c r="C41" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D41" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>183</v>
+      <c r="D41" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="E41" s="14" t="s">
+        <v>224</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>184</v>
+        <v>225</v>
       </c>
       <c r="G41" s="1">
         <v>2014</v>
       </c>
-      <c r="H41" s="6" t="s">
-        <v>185</v>
+      <c r="H41" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="I41" s="4">
-        <v>43934</v>
+        <v>43937</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>64</v>
@@ -3551,28 +3570,29 @@
       <c r="K41" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L41" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M41" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N41" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O41" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="P41" s="8" t="s">
-        <v>15</v>
-      </c>
+      <c r="L41" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M41" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="N41" s="21" t="s">
+        <v>265</v>
+      </c>
+      <c r="O41" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="P41" s="8"/>
       <c r="Q41" s="1" t="s">
-        <v>186</v>
+        <v>226</v>
+      </c>
+      <c r="R41">
+        <v>5.5</v>
       </c>
     </row>
     <row r="42" spans="1:18" ht="12.75">
       <c r="A42" s="1" t="s">
-        <v>187</v>
+        <v>15</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>23</v>
@@ -3581,22 +3601,22 @@
         <v>24</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>188</v>
-      </c>
-      <c r="E42" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>190</v>
+        <v>56</v>
+      </c>
+      <c r="E42" s="14" t="s">
+        <v>227</v>
+      </c>
+      <c r="F42" s="3" t="s">
+        <v>228</v>
       </c>
       <c r="G42" s="1">
-        <v>2012</v>
+        <v>2016</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>191</v>
+        <v>15</v>
       </c>
       <c r="I42" s="4">
-        <v>43934</v>
+        <v>43937</v>
       </c>
       <c r="J42" s="1" t="s">
         <v>64</v>
@@ -3605,27 +3625,22 @@
         <v>15</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="M42" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N42" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O42" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="P42" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>15</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="M42" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="N42" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="O42" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="P42" s="19"/>
     </row>
     <row r="43" spans="1:18" ht="12.75">
       <c r="A43" s="1" t="s">
-        <v>192</v>
+        <v>15</v>
       </c>
       <c r="B43" s="8" t="s">
         <v>23</v>
@@ -3634,22 +3649,22 @@
         <v>24</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E43" s="14" t="s">
-        <v>193</v>
+        <v>216</v>
+      </c>
+      <c r="E43" s="18" t="s">
+        <v>217</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>194</v>
+        <v>218</v>
       </c>
       <c r="G43" s="1">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="I43" s="4">
-        <v>43934</v>
+        <v>43937</v>
       </c>
       <c r="J43" s="1" t="s">
         <v>64</v>
@@ -3657,23 +3672,26 @@
       <c r="K43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L43" s="5" t="s">
-        <v>195</v>
+      <c r="L43" s="8" t="s">
+        <v>103</v>
       </c>
       <c r="M43" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N43" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="O43" s="8" t="s">
-        <v>15</v>
+      <c r="N43" s="24" t="s">
+        <v>260</v>
+      </c>
+      <c r="O43" s="24" t="s">
+        <v>260</v>
       </c>
       <c r="P43" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q43" s="1" t="s">
-        <v>186</v>
+      <c r="Q43" t="s">
+        <v>261</v>
+      </c>
+      <c r="R43">
+        <v>5.5</v>
       </c>
     </row>
     <row r="44" spans="1:18" ht="12.75">
@@ -3687,22 +3705,22 @@
         <v>24</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>197</v>
+        <v>61</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>108</v>
+        <v>63</v>
       </c>
       <c r="G44" s="1">
-        <v>2013</v>
+        <v>2011</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I44" s="4">
-        <v>43934</v>
+        <v>43915</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>64</v>
@@ -3710,81 +3728,81 @@
       <c r="K44" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L44" s="1" t="s">
+      <c r="L44" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="M44" s="8" t="s">
+      <c r="M44" s="21" t="s">
         <v>15</v>
       </c>
       <c r="N44" s="21" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="O44" s="21" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="P44" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q44" s="1" t="s">
-        <v>186</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="12.75">
-      <c r="A45" s="1" t="s">
-        <v>15</v>
+      <c r="A45" s="21" t="s">
+        <v>29</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>24</v>
+        <v>30</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>198</v>
+        <v>32</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>33</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>199</v>
+        <v>34</v>
       </c>
       <c r="G45" s="1">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>15</v>
+        <v>35</v>
       </c>
       <c r="I45" s="4">
-        <v>43935</v>
+        <v>43914</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="K45" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M45" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N45" t="s">
-        <v>247</v>
-      </c>
-      <c r="O45" s="1" t="s">
-        <v>247</v>
+        <v>21</v>
+      </c>
+      <c r="M45" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N45" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="O45" s="21" t="s">
+        <v>15</v>
       </c>
       <c r="P45" s="8" t="s">
         <v>15</v>
       </c>
       <c r="Q45" s="8" t="s">
-        <v>15</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="12.75">
       <c r="A46" s="1" t="s">
-        <v>200</v>
+        <v>170</v>
       </c>
       <c r="B46" s="8" t="s">
         <v>23</v>
@@ -3793,22 +3811,22 @@
         <v>24</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="E46" s="14" t="s">
-        <v>202</v>
+        <v>171</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="F46" s="1" t="s">
-        <v>203</v>
+        <v>173</v>
       </c>
       <c r="G46" s="1">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>204</v>
+        <v>174</v>
       </c>
       <c r="I46" s="4">
-        <v>43935</v>
+        <v>43928</v>
       </c>
       <c r="J46" s="1" t="s">
         <v>64</v>
@@ -3817,13 +3835,13 @@
         <v>15</v>
       </c>
       <c r="L46" s="1" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="M46" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N46" s="8" t="s">
-        <v>233</v>
+        <v>15</v>
       </c>
       <c r="O46" s="8" t="s">
         <v>15</v>
@@ -3832,12 +3850,12 @@
         <v>15</v>
       </c>
       <c r="Q46" s="8" t="s">
-        <v>15</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:18" ht="12.75">
       <c r="A47" s="1" t="s">
-        <v>15</v>
+        <v>160</v>
       </c>
       <c r="B47" s="8" t="s">
         <v>23</v>
@@ -3846,22 +3864,22 @@
         <v>24</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="E47" s="14" t="s">
-        <v>205</v>
+        <v>161</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="G47" s="1">
-        <v>2016</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>15</v>
+        <v>2013</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>164</v>
       </c>
       <c r="I47" s="4">
-        <v>43935</v>
+        <v>43923</v>
       </c>
       <c r="J47" s="1" t="s">
         <v>64</v>
@@ -3869,31 +3887,28 @@
       <c r="K47" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L47" s="5" t="s">
-        <v>159</v>
+      <c r="L47" s="8" t="s">
+        <v>301</v>
       </c>
       <c r="M47" s="8" t="s">
-        <v>249</v>
-      </c>
-      <c r="N47" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="N47" t="s">
         <v>15</v>
       </c>
       <c r="O47" s="2" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="P47" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q47" s="21" t="s">
-        <v>253</v>
-      </c>
-      <c r="R47">
-        <v>5.5</v>
+      <c r="Q47" s="8" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="48" spans="1:18" ht="12.75">
       <c r="A48" s="1" t="s">
-        <v>15</v>
+        <v>176</v>
       </c>
       <c r="B48" s="8" t="s">
         <v>23</v>
@@ -3902,22 +3917,22 @@
         <v>24</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>208</v>
+        <v>163</v>
       </c>
       <c r="G48" s="1">
-        <v>2017</v>
+        <v>2014</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>15</v>
+        <v>178</v>
       </c>
       <c r="I48" s="4">
-        <v>43935</v>
+        <v>43928</v>
       </c>
       <c r="J48" s="1" t="s">
         <v>64</v>
@@ -3925,31 +3940,28 @@
       <c r="K48" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L48" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="M48" s="16" t="s">
-        <v>251</v>
+      <c r="L48" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="M48" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="N48" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="O48" s="16" t="s">
-        <v>251</v>
+      <c r="O48" s="8" t="s">
+        <v>15</v>
       </c>
       <c r="P48" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q48" s="21" t="s">
-        <v>252</v>
-      </c>
-      <c r="R48">
-        <v>5.5</v>
+      <c r="Q48" s="8" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="49" spans="1:18" ht="12.75">
       <c r="A49" s="1" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="B49" s="8" t="s">
         <v>23</v>
@@ -3958,19 +3970,19 @@
         <v>24</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="E49" s="17" t="s">
-        <v>211</v>
+        <v>201</v>
+      </c>
+      <c r="E49" s="14" t="s">
+        <v>202</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="G49" s="1">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="I49" s="4">
         <v>43935</v>
@@ -3982,21 +3994,23 @@
         <v>15</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>214</v>
+        <v>112</v>
       </c>
       <c r="M49" s="8" t="s">
         <v>15</v>
       </c>
       <c r="N49" s="8" t="s">
-        <v>215</v>
+        <v>233</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>215</v>
+        <v>15</v>
       </c>
       <c r="P49" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q49" s="13"/>
+      <c r="Q49" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="50" spans="1:18" ht="12.75">
       <c r="A50" s="1" t="s">
@@ -4009,22 +4023,22 @@
         <v>24</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>216</v>
-      </c>
-      <c r="E50" s="18" t="s">
-        <v>217</v>
+        <v>66</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>67</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>218</v>
+        <v>68</v>
       </c>
       <c r="G50" s="1">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I50" s="4">
-        <v>43937</v>
+        <v>43915</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>64</v>
@@ -4032,26 +4046,23 @@
       <c r="K50" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L50" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M50" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="N50" s="24" t="s">
-        <v>260</v>
-      </c>
-      <c r="O50" s="24" t="s">
-        <v>260</v>
+      <c r="L50" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="M50" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N50" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="O50" s="21" t="s">
+        <v>233</v>
       </c>
       <c r="P50" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q50" t="s">
-        <v>261</v>
-      </c>
-      <c r="R50">
-        <v>5.5</v>
+      <c r="Q50" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="51" spans="1:18" ht="12.75">
@@ -4064,23 +4075,23 @@
       <c r="C51" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D51" s="20" t="s">
-        <v>219</v>
-      </c>
-      <c r="E51" s="14" t="s">
-        <v>220</v>
+      <c r="D51" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>92</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>221</v>
+        <v>93</v>
       </c>
       <c r="G51" s="1">
-        <v>2014</v>
+        <v>2010</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I51" s="4">
-        <v>43937</v>
+        <v>43917</v>
       </c>
       <c r="J51" s="1" t="s">
         <v>64</v>
@@ -4089,25 +4100,22 @@
         <v>15</v>
       </c>
       <c r="L51" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M51" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="N51" s="16" t="s">
-        <v>251</v>
-      </c>
-      <c r="O51" s="23" t="s">
-        <v>251</v>
+        <v>65</v>
+      </c>
+      <c r="M51" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="N51" s="21" t="s">
+        <v>235</v>
+      </c>
+      <c r="O51" s="21" t="s">
+        <v>235</v>
       </c>
       <c r="P51" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q51" s="21" t="s">
-        <v>248</v>
-      </c>
-      <c r="R51">
-        <v>5.5</v>
+      <c r="Q51" s="8" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="52" spans="1:18" ht="12.75">
@@ -4121,22 +4129,22 @@
         <v>24</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="E52" s="14" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>221</v>
+        <v>206</v>
       </c>
       <c r="G52" s="1">
-        <v>2011</v>
+        <v>2016</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I52" s="4">
-        <v>43937</v>
+        <v>43935</v>
       </c>
       <c r="J52" s="1" t="s">
         <v>64</v>
@@ -4144,23 +4152,23 @@
       <c r="K52" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L52" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="M52" s="22" t="s">
-        <v>262</v>
-      </c>
-      <c r="N52" s="22" t="s">
-        <v>262</v>
-      </c>
-      <c r="O52" s="22" t="s">
-        <v>262</v>
+      <c r="L52" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="M52" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="N52" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O52" s="8" t="s">
+        <v>249</v>
       </c>
       <c r="P52" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="Q52" s="22" t="s">
-        <v>263</v>
+      <c r="Q52" s="21" t="s">
+        <v>253</v>
       </c>
       <c r="R52">
         <v>5.5</v>
@@ -4176,23 +4184,23 @@
       <c r="C53" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="D53" s="15" t="s">
-        <v>223</v>
-      </c>
-      <c r="E53" s="14" t="s">
-        <v>224</v>
+      <c r="D53" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>101</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>225</v>
+        <v>102</v>
       </c>
       <c r="G53" s="1">
-        <v>2014</v>
+        <v>2012</v>
       </c>
       <c r="H53" s="1" t="s">
         <v>15</v>
       </c>
       <c r="I53" s="4">
-        <v>43937</v>
+        <v>43917</v>
       </c>
       <c r="J53" s="1" t="s">
         <v>64</v>
@@ -4200,134 +4208,142 @@
       <c r="K53" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L53" s="5" t="s">
-        <v>79</v>
+      <c r="L53" s="21" t="s">
+        <v>103</v>
       </c>
       <c r="M53" s="21" t="s">
-        <v>294</v>
+        <v>15</v>
       </c>
       <c r="N53" s="21" t="s">
-        <v>265</v>
+        <v>237</v>
       </c>
       <c r="O53" s="21" t="s">
-        <v>264</v>
-      </c>
-      <c r="P53" s="8"/>
+        <v>237</v>
+      </c>
+      <c r="P53" s="8" t="s">
+        <v>15</v>
+      </c>
       <c r="Q53" s="1" t="s">
-        <v>226</v>
-      </c>
-      <c r="R53">
-        <v>5.5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="54" spans="1:18" ht="12.75">
       <c r="A54" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B54" s="8" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C54" s="8" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E54" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="F54" s="3" t="s">
-        <v>228</v>
+        <v>15</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>17</v>
       </c>
       <c r="G54" s="1">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="I54" s="4">
-        <v>43937</v>
+        <v>43914</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="K54" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="L54" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="M54" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="N54" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="O54" s="19" t="s">
-        <v>229</v>
-      </c>
-      <c r="P54" s="19"/>
+        <v>21</v>
+      </c>
+      <c r="M54" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="N54" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="O54" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="P54" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q54" s="8" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R54">
+    <sortCondition ref="F2:F54"/>
+    <sortCondition ref="G2:G54"/>
+  </sortState>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="E3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
-    <hyperlink ref="E6" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
-    <hyperlink ref="E7" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
-    <hyperlink ref="E9" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="E10" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="E11" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="E13" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="H13" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="E14" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="E15" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="E16" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
-    <hyperlink ref="E17" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="E18" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
-    <hyperlink ref="E19" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
-    <hyperlink ref="E20" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
-    <hyperlink ref="E21" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
-    <hyperlink ref="E22" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
-    <hyperlink ref="E23" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
-    <hyperlink ref="E24" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
-    <hyperlink ref="E25" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
-    <hyperlink ref="E26" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
-    <hyperlink ref="E27" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
-    <hyperlink ref="E28" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
-    <hyperlink ref="E29" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
-    <hyperlink ref="E30" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
-    <hyperlink ref="H30" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
-    <hyperlink ref="E31" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
-    <hyperlink ref="H31" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
-    <hyperlink ref="E32" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
-    <hyperlink ref="E33" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
-    <hyperlink ref="H33" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
-    <hyperlink ref="E34" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
-    <hyperlink ref="E35" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
-    <hyperlink ref="E36" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
-    <hyperlink ref="H36" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
-    <hyperlink ref="E37" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
-    <hyperlink ref="E38" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
-    <hyperlink ref="E39" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
-    <hyperlink ref="E40" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
-    <hyperlink ref="E41" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
-    <hyperlink ref="H41" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
-    <hyperlink ref="E42" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
-    <hyperlink ref="E43" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
-    <hyperlink ref="E44" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
-    <hyperlink ref="E45" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
-    <hyperlink ref="E46" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
-    <hyperlink ref="E47" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
-    <hyperlink ref="E48" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
-    <hyperlink ref="E49" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
-    <hyperlink ref="E50" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
-    <hyperlink ref="E51" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
-    <hyperlink ref="E52" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
-    <hyperlink ref="E53" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
-    <hyperlink ref="E54" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
-    <hyperlink ref="E5" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
-    <hyperlink ref="E12" r:id="rId58" xr:uid="{0896B016-0F4A-4186-939D-3E08BDF72736}"/>
+    <hyperlink ref="E54" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="E30" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="E45" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="E10" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="E31" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="E21" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="E44" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="E50" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="E33" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="H33" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="E4" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="E5" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="E25" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="E34" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="E51" r:id="rId15" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="E26" r:id="rId16" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="E13" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="E53" r:id="rId18" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="E9" r:id="rId19" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="E17" r:id="rId20" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="E35" r:id="rId21" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="E28" r:id="rId22" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="E3" r:id="rId23" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="E22" r:id="rId24" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="E38" r:id="rId25" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="E16" r:id="rId26" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="E12" r:id="rId27" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="H12" r:id="rId28" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="E23" r:id="rId29" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="H23" r:id="rId30" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="E40" r:id="rId31" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="E19" r:id="rId32" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="H19" r:id="rId33" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="E39" r:id="rId34" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="E36" r:id="rId35" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="E47" r:id="rId36" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="H47" r:id="rId37" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="E11" r:id="rId38" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="E46" r:id="rId39" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="E48" r:id="rId40" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="E27" r:id="rId41" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="E14" r:id="rId42" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
+    <hyperlink ref="H14" r:id="rId43" xr:uid="{00000000-0004-0000-0000-00002E000000}"/>
+    <hyperlink ref="E29" r:id="rId44" xr:uid="{00000000-0004-0000-0000-00002F000000}"/>
+    <hyperlink ref="E24" r:id="rId45" xr:uid="{00000000-0004-0000-0000-000030000000}"/>
+    <hyperlink ref="E18" r:id="rId46" xr:uid="{00000000-0004-0000-0000-000031000000}"/>
+    <hyperlink ref="E6" r:id="rId47" xr:uid="{00000000-0004-0000-0000-000034000000}"/>
+    <hyperlink ref="E49" r:id="rId48" xr:uid="{00000000-0004-0000-0000-000035000000}"/>
+    <hyperlink ref="E52" r:id="rId49" xr:uid="{00000000-0004-0000-0000-000036000000}"/>
+    <hyperlink ref="E20" r:id="rId50" xr:uid="{00000000-0004-0000-0000-000037000000}"/>
+    <hyperlink ref="E2" r:id="rId51" xr:uid="{00000000-0004-0000-0000-000038000000}"/>
+    <hyperlink ref="E43" r:id="rId52" xr:uid="{00000000-0004-0000-0000-000039000000}"/>
+    <hyperlink ref="E8" r:id="rId53" xr:uid="{00000000-0004-0000-0000-00003A000000}"/>
+    <hyperlink ref="E7" r:id="rId54" xr:uid="{00000000-0004-0000-0000-00003B000000}"/>
+    <hyperlink ref="E41" r:id="rId55" xr:uid="{00000000-0004-0000-0000-00003C000000}"/>
+    <hyperlink ref="E42" r:id="rId56" xr:uid="{00000000-0004-0000-0000-00003D000000}"/>
+    <hyperlink ref="E37" r:id="rId57" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="E32" r:id="rId58" xr:uid="{0896B016-0F4A-4186-939D-3E08BDF72736}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId59"/>

</xml_diff>